<commit_message>
Justering protokoll rökna ut övningar och avdrag
</commit_message>
<xml_diff>
--- a/mallar/Protokoll/Protokoll_2019_lag_sv-r_mellan(mall).xlsx
+++ b/mallar/Protokoll/Protokoll_2019_lag_sv-r_mellan(mall).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\episerver\voltige\VoltigeClosedXML\mallar\Protokoll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E9B558-01B7-4EEB-97A9-C0F7A7189254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D555A08D-8DC5-412B-8A2C-041C63AC520C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9982" yWindow="5483" windowWidth="16200" windowHeight="9397" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="27" r:id="rId1"/>
@@ -1734,7 +1734,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="267">
+  <cellXfs count="271">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2176,7 +2176,112 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="42" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="50" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="54" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2241,9 +2346,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -2262,122 +2364,35 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="42" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2389,21 +2404,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -2422,6 +2422,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
@@ -2437,27 +2443,25 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Dezimal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -3776,8 +3780,8 @@
         <v>14</v>
       </c>
       <c r="B4" s="148"/>
-      <c r="C4" s="230"/>
-      <c r="D4" s="230"/>
+      <c r="C4" s="175"/>
+      <c r="D4" s="175"/>
       <c r="E4" s="149"/>
       <c r="G4" s="142"/>
       <c r="H4" s="143" t="s">
@@ -3792,9 +3796,9 @@
         <v>15</v>
       </c>
       <c r="B5" s="150"/>
-      <c r="C5" s="227"/>
-      <c r="D5" s="227"/>
-      <c r="E5" s="227"/>
+      <c r="C5" s="172"/>
+      <c r="D5" s="172"/>
+      <c r="E5" s="172"/>
       <c r="G5" s="142"/>
       <c r="H5" s="143" t="s">
         <v>13</v>
@@ -3808,9 +3812,9 @@
         <v>16</v>
       </c>
       <c r="B6" s="150"/>
-      <c r="C6" s="227"/>
-      <c r="D6" s="227"/>
-      <c r="E6" s="227"/>
+      <c r="C6" s="172"/>
+      <c r="D6" s="172"/>
+      <c r="E6" s="172"/>
       <c r="G6" s="140" t="s">
         <v>18</v>
       </c>
@@ -3827,77 +3831,77 @@
       <c r="G7" s="148" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="231"/>
-      <c r="I7" s="232"/>
-      <c r="J7" s="232"/>
-      <c r="K7" s="233"/>
+      <c r="H7" s="176"/>
+      <c r="I7" s="177"/>
+      <c r="J7" s="177"/>
+      <c r="K7" s="178"/>
     </row>
     <row r="8" spans="1:12" s="140" customFormat="1" ht="17.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="148" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="148"/>
-      <c r="C8" s="231"/>
-      <c r="D8" s="231"/>
-      <c r="E8" s="231"/>
+      <c r="C8" s="176"/>
+      <c r="D8" s="176"/>
+      <c r="E8" s="176"/>
       <c r="G8" s="150" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="227"/>
-      <c r="I8" s="228"/>
-      <c r="J8" s="228"/>
-      <c r="K8" s="229"/>
+      <c r="H8" s="172"/>
+      <c r="I8" s="173"/>
+      <c r="J8" s="173"/>
+      <c r="K8" s="174"/>
     </row>
     <row r="9" spans="1:12" s="140" customFormat="1" ht="17.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="150" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="150"/>
-      <c r="C9" s="227"/>
-      <c r="D9" s="227"/>
-      <c r="E9" s="227"/>
+      <c r="C9" s="172"/>
+      <c r="D9" s="172"/>
+      <c r="E9" s="172"/>
       <c r="G9" s="150" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="227"/>
-      <c r="I9" s="228"/>
-      <c r="J9" s="228"/>
-      <c r="K9" s="229"/>
+      <c r="H9" s="172"/>
+      <c r="I9" s="173"/>
+      <c r="J9" s="173"/>
+      <c r="K9" s="174"/>
     </row>
     <row r="10" spans="1:12" s="140" customFormat="1" ht="17.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="150" t="s">
         <v>65</v>
       </c>
       <c r="B10" s="150"/>
-      <c r="C10" s="227"/>
-      <c r="D10" s="227"/>
-      <c r="E10" s="227"/>
+      <c r="C10" s="172"/>
+      <c r="D10" s="172"/>
+      <c r="E10" s="172"/>
       <c r="G10" s="150" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="227"/>
-      <c r="I10" s="228"/>
-      <c r="J10" s="228"/>
-      <c r="K10" s="229"/>
+      <c r="H10" s="172"/>
+      <c r="I10" s="173"/>
+      <c r="J10" s="173"/>
+      <c r="K10" s="174"/>
     </row>
     <row r="11" spans="1:12" s="140" customFormat="1" ht="17.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G11" s="150" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="227"/>
-      <c r="I11" s="228"/>
-      <c r="J11" s="228"/>
-      <c r="K11" s="229"/>
+      <c r="H11" s="172"/>
+      <c r="I11" s="173"/>
+      <c r="J11" s="173"/>
+      <c r="K11" s="174"/>
     </row>
     <row r="12" spans="1:12" s="140" customFormat="1" ht="17.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="154"/>
       <c r="G12" s="150" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="227"/>
-      <c r="I12" s="228"/>
-      <c r="J12" s="228"/>
-      <c r="K12" s="229"/>
+      <c r="H12" s="172"/>
+      <c r="I12" s="173"/>
+      <c r="J12" s="173"/>
+      <c r="K12" s="174"/>
     </row>
     <row r="13" spans="1:12" s="140" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C13" s="154"/>
@@ -3915,86 +3919,86 @@
       <c r="E14" s="157"/>
       <c r="F14" s="157"/>
       <c r="G14" s="140"/>
-      <c r="H14" s="202" t="s">
+      <c r="H14" s="179" t="s">
         <v>30</v>
       </c>
-      <c r="I14" s="203"/>
-      <c r="J14" s="204" t="s">
+      <c r="I14" s="180"/>
+      <c r="J14" s="181" t="s">
         <v>66</v>
       </c>
-      <c r="K14" s="205"/>
-      <c r="L14" s="206"/>
+      <c r="K14" s="182"/>
+      <c r="L14" s="183"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="207" t="s">
+      <c r="A15" s="184" t="s">
         <v>124</v>
       </c>
-      <c r="B15" s="211" t="s">
+      <c r="B15" s="188" t="s">
         <v>125</v>
       </c>
-      <c r="C15" s="212"/>
-      <c r="D15" s="212"/>
-      <c r="E15" s="212"/>
-      <c r="F15" s="212"/>
-      <c r="G15" s="212"/>
-      <c r="H15" s="215"/>
-      <c r="I15" s="216"/>
-      <c r="J15" s="221" t="s">
+      <c r="C15" s="189"/>
+      <c r="D15" s="189"/>
+      <c r="E15" s="189"/>
+      <c r="F15" s="189"/>
+      <c r="G15" s="189"/>
+      <c r="H15" s="192"/>
+      <c r="I15" s="193"/>
+      <c r="J15" s="198" t="s">
         <v>126</v>
       </c>
-      <c r="K15" s="223">
+      <c r="K15" s="201">
         <f>SUM(B20:G20)/6</f>
         <v>0</v>
       </c>
-      <c r="L15" s="193">
+      <c r="L15" s="204">
         <f>ROUND(K15*0.6,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="208"/>
-      <c r="B16" s="213"/>
-      <c r="C16" s="214"/>
-      <c r="D16" s="214"/>
-      <c r="E16" s="214"/>
-      <c r="F16" s="214"/>
-      <c r="G16" s="214"/>
-      <c r="H16" s="217"/>
-      <c r="I16" s="218"/>
-      <c r="J16" s="200"/>
-      <c r="K16" s="224"/>
-      <c r="L16" s="172"/>
+      <c r="A16" s="185"/>
+      <c r="B16" s="190"/>
+      <c r="C16" s="191"/>
+      <c r="D16" s="191"/>
+      <c r="E16" s="191"/>
+      <c r="F16" s="191"/>
+      <c r="G16" s="191"/>
+      <c r="H16" s="194"/>
+      <c r="I16" s="195"/>
+      <c r="J16" s="199"/>
+      <c r="K16" s="202"/>
+      <c r="L16" s="205"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="208"/>
-      <c r="B17" s="213"/>
-      <c r="C17" s="214"/>
-      <c r="D17" s="214"/>
-      <c r="E17" s="214"/>
-      <c r="F17" s="214"/>
-      <c r="G17" s="214"/>
-      <c r="H17" s="217"/>
-      <c r="I17" s="218"/>
-      <c r="J17" s="200"/>
-      <c r="K17" s="224"/>
-      <c r="L17" s="172"/>
+      <c r="A17" s="185"/>
+      <c r="B17" s="190"/>
+      <c r="C17" s="191"/>
+      <c r="D17" s="191"/>
+      <c r="E17" s="191"/>
+      <c r="F17" s="191"/>
+      <c r="G17" s="191"/>
+      <c r="H17" s="194"/>
+      <c r="I17" s="195"/>
+      <c r="J17" s="199"/>
+      <c r="K17" s="202"/>
+      <c r="L17" s="205"/>
     </row>
     <row r="18" spans="1:12" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="208"/>
-      <c r="B18" s="213"/>
-      <c r="C18" s="214"/>
-      <c r="D18" s="214"/>
-      <c r="E18" s="214"/>
-      <c r="F18" s="214"/>
-      <c r="G18" s="214"/>
-      <c r="H18" s="217"/>
-      <c r="I18" s="218"/>
-      <c r="J18" s="200"/>
-      <c r="K18" s="224"/>
-      <c r="L18" s="172"/>
+      <c r="A18" s="185"/>
+      <c r="B18" s="190"/>
+      <c r="C18" s="191"/>
+      <c r="D18" s="191"/>
+      <c r="E18" s="191"/>
+      <c r="F18" s="191"/>
+      <c r="G18" s="191"/>
+      <c r="H18" s="194"/>
+      <c r="I18" s="195"/>
+      <c r="J18" s="199"/>
+      <c r="K18" s="202"/>
+      <c r="L18" s="205"/>
     </row>
     <row r="19" spans="1:12" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="209"/>
+      <c r="A19" s="186"/>
       <c r="B19" s="158" t="s">
         <v>127</v>
       </c>
@@ -4013,14 +4017,14 @@
       <c r="G19" s="161" t="s">
         <v>132</v>
       </c>
-      <c r="H19" s="217"/>
-      <c r="I19" s="218"/>
-      <c r="J19" s="200"/>
-      <c r="K19" s="224"/>
-      <c r="L19" s="172"/>
+      <c r="H19" s="194"/>
+      <c r="I19" s="195"/>
+      <c r="J19" s="199"/>
+      <c r="K19" s="202"/>
+      <c r="L19" s="205"/>
     </row>
     <row r="20" spans="1:12" ht="28.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="210"/>
+      <c r="A20" s="187"/>
       <c r="B20" s="162">
         <v>0</v>
       </c>
@@ -4029,67 +4033,67 @@
       <c r="E20" s="163"/>
       <c r="F20" s="163"/>
       <c r="G20" s="164"/>
-      <c r="H20" s="219"/>
-      <c r="I20" s="220"/>
-      <c r="J20" s="222"/>
-      <c r="K20" s="225"/>
-      <c r="L20" s="226"/>
+      <c r="H20" s="196"/>
+      <c r="I20" s="197"/>
+      <c r="J20" s="200"/>
+      <c r="K20" s="203"/>
+      <c r="L20" s="206"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="176" t="s">
+      <c r="A21" s="210" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="179" t="s">
+      <c r="B21" s="213" t="s">
         <v>133</v>
       </c>
-      <c r="C21" s="179"/>
-      <c r="D21" s="179"/>
-      <c r="E21" s="179"/>
-      <c r="F21" s="179"/>
-      <c r="G21" s="179"/>
-      <c r="H21" s="182"/>
-      <c r="I21" s="183"/>
-      <c r="J21" s="188" t="s">
+      <c r="C21" s="213"/>
+      <c r="D21" s="213"/>
+      <c r="E21" s="213"/>
+      <c r="F21" s="213"/>
+      <c r="G21" s="213"/>
+      <c r="H21" s="216"/>
+      <c r="I21" s="217"/>
+      <c r="J21" s="222" t="s">
         <v>10</v>
       </c>
-      <c r="K21" s="191">
-        <v>0</v>
-      </c>
-      <c r="L21" s="193">
+      <c r="K21" s="225">
+        <v>0</v>
+      </c>
+      <c r="L21" s="204">
         <f>IF((K21-K24)&gt;=0,ROUND((K21-K24)*0.25,3),0.000000000001)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="177"/>
-      <c r="B22" s="180"/>
-      <c r="C22" s="180"/>
-      <c r="D22" s="180"/>
-      <c r="E22" s="180"/>
-      <c r="F22" s="180"/>
-      <c r="G22" s="180"/>
-      <c r="H22" s="184"/>
-      <c r="I22" s="185"/>
-      <c r="J22" s="189"/>
-      <c r="K22" s="192"/>
-      <c r="L22" s="172"/>
+      <c r="A22" s="211"/>
+      <c r="B22" s="214"/>
+      <c r="C22" s="214"/>
+      <c r="D22" s="214"/>
+      <c r="E22" s="214"/>
+      <c r="F22" s="214"/>
+      <c r="G22" s="214"/>
+      <c r="H22" s="218"/>
+      <c r="I22" s="219"/>
+      <c r="J22" s="223"/>
+      <c r="K22" s="226"/>
+      <c r="L22" s="205"/>
     </row>
     <row r="23" spans="1:12" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="177"/>
-      <c r="B23" s="181"/>
-      <c r="C23" s="181"/>
-      <c r="D23" s="181"/>
-      <c r="E23" s="181"/>
-      <c r="F23" s="181"/>
-      <c r="G23" s="180"/>
-      <c r="H23" s="184"/>
-      <c r="I23" s="185"/>
-      <c r="J23" s="189"/>
-      <c r="K23" s="192"/>
-      <c r="L23" s="172"/>
+      <c r="A23" s="211"/>
+      <c r="B23" s="215"/>
+      <c r="C23" s="215"/>
+      <c r="D23" s="215"/>
+      <c r="E23" s="215"/>
+      <c r="F23" s="215"/>
+      <c r="G23" s="214"/>
+      <c r="H23" s="218"/>
+      <c r="I23" s="219"/>
+      <c r="J23" s="223"/>
+      <c r="K23" s="226"/>
+      <c r="L23" s="205"/>
     </row>
     <row r="24" spans="1:12" ht="28.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="178"/>
+      <c r="A24" s="212"/>
       <c r="B24" s="165" t="s">
         <v>134</v>
       </c>
@@ -4108,42 +4112,42 @@
       <c r="G24" s="166">
         <v>0</v>
       </c>
-      <c r="H24" s="186"/>
-      <c r="I24" s="187"/>
-      <c r="J24" s="190"/>
+      <c r="H24" s="220"/>
+      <c r="I24" s="221"/>
+      <c r="J24" s="224"/>
       <c r="K24" s="167">
         <f>SUM(C24:G24)</f>
         <v>0</v>
       </c>
-      <c r="L24" s="173"/>
+      <c r="L24" s="207"/>
     </row>
     <row r="25" spans="1:12" ht="67.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="176" t="s">
+      <c r="A25" s="210" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="179" t="s">
+      <c r="B25" s="213" t="s">
         <v>135</v>
       </c>
-      <c r="C25" s="194"/>
-      <c r="D25" s="194"/>
-      <c r="E25" s="194"/>
-      <c r="F25" s="194"/>
-      <c r="G25" s="195"/>
-      <c r="H25" s="196"/>
-      <c r="I25" s="197"/>
-      <c r="J25" s="200" t="s">
+      <c r="C25" s="227"/>
+      <c r="D25" s="227"/>
+      <c r="E25" s="227"/>
+      <c r="F25" s="227"/>
+      <c r="G25" s="228"/>
+      <c r="H25" s="229"/>
+      <c r="I25" s="230"/>
+      <c r="J25" s="199" t="s">
         <v>136</v>
       </c>
       <c r="K25" s="168">
         <v>0</v>
       </c>
-      <c r="L25" s="172">
+      <c r="L25" s="205">
         <f>IF((K25-K26)&gt;=0,ROUND((K25-K26)*0.15,3),0.00000000001)</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="28.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="178"/>
+      <c r="A26" s="212"/>
       <c r="B26" s="169" t="s">
         <v>134</v>
       </c>
@@ -4160,14 +4164,14 @@
         <v>0</v>
       </c>
       <c r="G26" s="166"/>
-      <c r="H26" s="198"/>
-      <c r="I26" s="199"/>
-      <c r="J26" s="201"/>
+      <c r="H26" s="231"/>
+      <c r="I26" s="232"/>
+      <c r="J26" s="233"/>
       <c r="K26" s="167">
         <f>SUM(C26:G26)</f>
         <v>0</v>
       </c>
-      <c r="L26" s="173"/>
+      <c r="L26" s="207"/>
     </row>
     <row r="27" spans="1:12" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="44"/>
@@ -4185,11 +4189,11 @@
         <v>12</v>
       </c>
       <c r="J28" s="46"/>
-      <c r="K28" s="174">
+      <c r="K28" s="208">
         <f>SUM(L15:L25)</f>
         <v>0</v>
       </c>
-      <c r="L28" s="175"/>
+      <c r="L28" s="209"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="171" t="s">
@@ -4211,6 +4215,26 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="L25:L26"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="B21:G23"/>
+    <mergeCell ref="H21:I24"/>
+    <mergeCell ref="J21:J24"/>
+    <mergeCell ref="K21:K23"/>
+    <mergeCell ref="L21:L24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="H25:I26"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="B15:G18"/>
+    <mergeCell ref="H15:I20"/>
+    <mergeCell ref="J15:J20"/>
+    <mergeCell ref="K15:K20"/>
+    <mergeCell ref="L15:L20"/>
     <mergeCell ref="H12:K12"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:E5"/>
@@ -4223,26 +4247,6 @@
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="H10:K10"/>
     <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="B15:G18"/>
-    <mergeCell ref="H15:I20"/>
-    <mergeCell ref="J15:J20"/>
-    <mergeCell ref="K15:K20"/>
-    <mergeCell ref="L15:L20"/>
-    <mergeCell ref="L25:L26"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="B21:G23"/>
-    <mergeCell ref="H21:I24"/>
-    <mergeCell ref="J21:J24"/>
-    <mergeCell ref="K21:K23"/>
-    <mergeCell ref="L21:L24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="H25:I26"/>
-    <mergeCell ref="J25:J26"/>
   </mergeCells>
   <pageMargins left="0.47244094488188981" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4324,10 +4328,10 @@
         <v>15</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" s="234"/>
-      <c r="D5" s="234"/>
-      <c r="E5" s="234"/>
-      <c r="F5" s="234"/>
+      <c r="C5" s="241"/>
+      <c r="D5" s="241"/>
+      <c r="E5" s="241"/>
+      <c r="F5" s="241"/>
       <c r="H5" s="9"/>
       <c r="I5" s="13" t="s">
         <v>13</v>
@@ -4341,10 +4345,10 @@
         <v>16</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="234"/>
-      <c r="D6" s="234"/>
-      <c r="E6" s="234"/>
-      <c r="F6" s="234"/>
+      <c r="C6" s="241"/>
+      <c r="D6" s="241"/>
+      <c r="E6" s="241"/>
+      <c r="F6" s="241"/>
       <c r="H6" s="1" t="s">
         <v>18</v>
       </c>
@@ -4361,79 +4365,79 @@
       <c r="H7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="239"/>
-      <c r="J7" s="240"/>
-      <c r="K7" s="240"/>
-      <c r="L7" s="241"/>
+      <c r="I7" s="244"/>
+      <c r="J7" s="245"/>
+      <c r="K7" s="245"/>
+      <c r="L7" s="246"/>
     </row>
     <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="239"/>
-      <c r="D8" s="239"/>
-      <c r="E8" s="239"/>
-      <c r="F8" s="239"/>
+      <c r="C8" s="244"/>
+      <c r="D8" s="244"/>
+      <c r="E8" s="244"/>
+      <c r="F8" s="244"/>
       <c r="H8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="234"/>
-      <c r="J8" s="235"/>
-      <c r="K8" s="235"/>
-      <c r="L8" s="236"/>
+      <c r="I8" s="241"/>
+      <c r="J8" s="242"/>
+      <c r="K8" s="242"/>
+      <c r="L8" s="243"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="12"/>
-      <c r="C9" s="234"/>
-      <c r="D9" s="234"/>
-      <c r="E9" s="234"/>
-      <c r="F9" s="234"/>
+      <c r="C9" s="241"/>
+      <c r="D9" s="241"/>
+      <c r="E9" s="241"/>
+      <c r="F9" s="241"/>
       <c r="H9" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="234"/>
-      <c r="J9" s="235"/>
-      <c r="K9" s="235"/>
-      <c r="L9" s="236"/>
+      <c r="I9" s="241"/>
+      <c r="J9" s="242"/>
+      <c r="K9" s="242"/>
+      <c r="L9" s="243"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>65</v>
       </c>
       <c r="B10" s="12"/>
-      <c r="C10" s="234"/>
-      <c r="D10" s="234"/>
-      <c r="E10" s="234"/>
-      <c r="F10" s="234"/>
+      <c r="C10" s="241"/>
+      <c r="D10" s="241"/>
+      <c r="E10" s="241"/>
+      <c r="F10" s="241"/>
       <c r="H10" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="234"/>
-      <c r="J10" s="235"/>
-      <c r="K10" s="235"/>
-      <c r="L10" s="236"/>
+      <c r="I10" s="241"/>
+      <c r="J10" s="242"/>
+      <c r="K10" s="242"/>
+      <c r="L10" s="243"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="234"/>
-      <c r="J11" s="235"/>
-      <c r="K11" s="235"/>
-      <c r="L11" s="236"/>
+      <c r="I11" s="241"/>
+      <c r="J11" s="242"/>
+      <c r="K11" s="242"/>
+      <c r="L11" s="243"/>
     </row>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H12" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="234"/>
-      <c r="J12" s="235"/>
-      <c r="K12" s="235"/>
-      <c r="L12" s="236"/>
+      <c r="I12" s="241"/>
+      <c r="J12" s="242"/>
+      <c r="K12" s="242"/>
+      <c r="L12" s="243"/>
     </row>
     <row r="13" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15"/>
@@ -4463,12 +4467,12 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="244"/>
-      <c r="B15" s="245" t="s">
+      <c r="A15" s="234"/>
+      <c r="B15" s="235" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="238"/>
-      <c r="D15" s="238"/>
+      <c r="C15" s="236"/>
+      <c r="D15" s="236"/>
       <c r="E15" s="18"/>
       <c r="F15" s="128"/>
       <c r="G15" s="128"/>
@@ -4482,12 +4486,12 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="244"/>
+      <c r="A16" s="234"/>
       <c r="B16" s="237" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="238"/>
-      <c r="D16" s="238"/>
+      <c r="C16" s="236"/>
+      <c r="D16" s="236"/>
       <c r="E16" s="18"/>
       <c r="F16" s="128"/>
       <c r="G16" s="128"/>
@@ -4504,8 +4508,8 @@
       <c r="B17" s="237" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="238"/>
-      <c r="D17" s="238"/>
+      <c r="C17" s="236"/>
+      <c r="D17" s="236"/>
       <c r="E17" s="18"/>
       <c r="F17" s="128"/>
       <c r="G17" s="128"/>
@@ -4519,11 +4523,11 @@
       </c>
     </row>
     <row r="18" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="242" t="s">
+      <c r="B18" s="247" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="243"/>
-      <c r="D18" s="243"/>
+      <c r="C18" s="248"/>
+      <c r="D18" s="248"/>
       <c r="E18" s="18"/>
       <c r="F18" s="128"/>
       <c r="G18" s="128"/>
@@ -4540,8 +4544,8 @@
       <c r="B19" s="237" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="238"/>
-      <c r="D19" s="238"/>
+      <c r="C19" s="236"/>
+      <c r="D19" s="236"/>
       <c r="E19" s="20"/>
       <c r="F19" s="128"/>
       <c r="G19" s="128"/>
@@ -4591,12 +4595,12 @@
       </c>
     </row>
     <row r="22" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="246" t="s">
+      <c r="B22" s="238" t="s">
         <v>115</v>
       </c>
-      <c r="C22" s="247"/>
-      <c r="D22" s="247"/>
-      <c r="E22" s="248"/>
+      <c r="C22" s="239"/>
+      <c r="D22" s="239"/>
+      <c r="E22" s="240"/>
       <c r="F22" s="128"/>
       <c r="G22" s="128"/>
       <c r="H22" s="128"/>
@@ -4720,11 +4724,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B22:E22"/>
     <mergeCell ref="I12:L12"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="C8:F8"/>
@@ -4738,6 +4737,11 @@
     <mergeCell ref="I10:L10"/>
     <mergeCell ref="I11:L11"/>
     <mergeCell ref="C6:F6"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B22:E22"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4820,10 +4824,10 @@
         <v>15</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" s="234"/>
-      <c r="D5" s="234"/>
-      <c r="E5" s="234"/>
-      <c r="F5" s="234"/>
+      <c r="C5" s="241"/>
+      <c r="D5" s="241"/>
+      <c r="E5" s="241"/>
+      <c r="F5" s="241"/>
       <c r="H5" s="9"/>
       <c r="I5" s="13" t="s">
         <v>13</v>
@@ -4837,10 +4841,10 @@
         <v>16</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="234"/>
-      <c r="D6" s="234"/>
-      <c r="E6" s="234"/>
-      <c r="F6" s="234"/>
+      <c r="C6" s="241"/>
+      <c r="D6" s="241"/>
+      <c r="E6" s="241"/>
+      <c r="F6" s="241"/>
       <c r="H6" s="1" t="s">
         <v>18</v>
       </c>
@@ -4857,80 +4861,80 @@
       <c r="H7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="239"/>
-      <c r="J7" s="240"/>
-      <c r="K7" s="240"/>
-      <c r="L7" s="241"/>
+      <c r="I7" s="244"/>
+      <c r="J7" s="245"/>
+      <c r="K7" s="245"/>
+      <c r="L7" s="246"/>
     </row>
     <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="239"/>
-      <c r="D8" s="239"/>
-      <c r="E8" s="239"/>
-      <c r="F8" s="239"/>
+      <c r="C8" s="244"/>
+      <c r="D8" s="244"/>
+      <c r="E8" s="244"/>
+      <c r="F8" s="244"/>
       <c r="H8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="234"/>
-      <c r="J8" s="235"/>
-      <c r="K8" s="235"/>
-      <c r="L8" s="236"/>
+      <c r="I8" s="241"/>
+      <c r="J8" s="242"/>
+      <c r="K8" s="242"/>
+      <c r="L8" s="243"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="12"/>
-      <c r="C9" s="234"/>
-      <c r="D9" s="234"/>
-      <c r="E9" s="234"/>
-      <c r="F9" s="234"/>
+      <c r="C9" s="241"/>
+      <c r="D9" s="241"/>
+      <c r="E9" s="241"/>
+      <c r="F9" s="241"/>
       <c r="H9" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="234"/>
-      <c r="J9" s="235"/>
-      <c r="K9" s="235"/>
-      <c r="L9" s="236"/>
+      <c r="I9" s="241"/>
+      <c r="J9" s="242"/>
+      <c r="K9" s="242"/>
+      <c r="L9" s="243"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>65</v>
       </c>
       <c r="B10" s="12"/>
-      <c r="C10" s="234"/>
-      <c r="D10" s="234"/>
-      <c r="E10" s="234"/>
-      <c r="F10" s="234"/>
+      <c r="C10" s="241"/>
+      <c r="D10" s="241"/>
+      <c r="E10" s="241"/>
+      <c r="F10" s="241"/>
       <c r="H10" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="234"/>
-      <c r="J10" s="235"/>
-      <c r="K10" s="235"/>
-      <c r="L10" s="236"/>
+      <c r="I10" s="241"/>
+      <c r="J10" s="242"/>
+      <c r="K10" s="242"/>
+      <c r="L10" s="243"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="234"/>
-      <c r="J11" s="235"/>
-      <c r="K11" s="235"/>
-      <c r="L11" s="236"/>
+      <c r="I11" s="241"/>
+      <c r="J11" s="242"/>
+      <c r="K11" s="242"/>
+      <c r="L11" s="243"/>
     </row>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="14"/>
       <c r="H12" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="234"/>
-      <c r="J12" s="235"/>
-      <c r="K12" s="235"/>
-      <c r="L12" s="236"/>
+      <c r="I12" s="241"/>
+      <c r="J12" s="242"/>
+      <c r="K12" s="242"/>
+      <c r="L12" s="243"/>
     </row>
     <row r="13" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15"/>
@@ -4960,12 +4964,12 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="244"/>
-      <c r="B15" s="245" t="s">
+      <c r="A15" s="234"/>
+      <c r="B15" s="235" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="238"/>
-      <c r="D15" s="238"/>
+      <c r="C15" s="236"/>
+      <c r="D15" s="236"/>
       <c r="E15" s="18"/>
       <c r="F15" s="128"/>
       <c r="G15" s="128"/>
@@ -4979,12 +4983,12 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="244"/>
+      <c r="A16" s="234"/>
       <c r="B16" s="237" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="238"/>
-      <c r="D16" s="238"/>
+      <c r="C16" s="236"/>
+      <c r="D16" s="236"/>
       <c r="E16" s="18"/>
       <c r="F16" s="128"/>
       <c r="G16" s="128"/>
@@ -5001,8 +5005,8 @@
       <c r="B17" s="237" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="238"/>
-      <c r="D17" s="238"/>
+      <c r="C17" s="236"/>
+      <c r="D17" s="236"/>
       <c r="E17" s="18"/>
       <c r="F17" s="128"/>
       <c r="G17" s="128"/>
@@ -5019,8 +5023,8 @@
       <c r="B18" s="251" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="238"/>
-      <c r="D18" s="238"/>
+      <c r="C18" s="236"/>
+      <c r="D18" s="236"/>
       <c r="E18" s="18"/>
       <c r="F18" s="128"/>
       <c r="G18" s="128"/>
@@ -5034,11 +5038,11 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="242" t="s">
+      <c r="B19" s="247" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="243"/>
-      <c r="D19" s="243"/>
+      <c r="C19" s="248"/>
+      <c r="D19" s="248"/>
       <c r="E19" s="20"/>
       <c r="F19" s="128"/>
       <c r="G19" s="128"/>
@@ -5055,8 +5059,8 @@
       <c r="B20" s="237" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="238"/>
-      <c r="D20" s="238"/>
+      <c r="C20" s="236"/>
+      <c r="D20" s="236"/>
       <c r="E20" s="18"/>
       <c r="F20" s="128"/>
       <c r="G20" s="128"/>
@@ -5221,13 +5225,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="I12:L12"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="I7:L7"/>
     <mergeCell ref="C6:F6"/>
@@ -5240,6 +5237,13 @@
     <mergeCell ref="I10:L10"/>
     <mergeCell ref="I11:L11"/>
     <mergeCell ref="C9:F9"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5322,10 +5326,10 @@
         <v>15</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" s="234"/>
-      <c r="D5" s="234"/>
-      <c r="E5" s="234"/>
-      <c r="F5" s="234"/>
+      <c r="C5" s="241"/>
+      <c r="D5" s="241"/>
+      <c r="E5" s="241"/>
+      <c r="F5" s="241"/>
       <c r="H5" s="9"/>
       <c r="I5" s="13" t="s">
         <v>13</v>
@@ -5339,10 +5343,10 @@
         <v>16</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="234"/>
-      <c r="D6" s="234"/>
-      <c r="E6" s="234"/>
-      <c r="F6" s="234"/>
+      <c r="C6" s="241"/>
+      <c r="D6" s="241"/>
+      <c r="E6" s="241"/>
+      <c r="F6" s="241"/>
       <c r="H6" s="1" t="s">
         <v>18</v>
       </c>
@@ -5359,80 +5363,80 @@
       <c r="H7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="239"/>
-      <c r="J7" s="240"/>
-      <c r="K7" s="240"/>
-      <c r="L7" s="240"/>
+      <c r="I7" s="244"/>
+      <c r="J7" s="245"/>
+      <c r="K7" s="245"/>
+      <c r="L7" s="245"/>
     </row>
     <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="239"/>
-      <c r="D8" s="239"/>
-      <c r="E8" s="239"/>
-      <c r="F8" s="239"/>
+      <c r="C8" s="244"/>
+      <c r="D8" s="244"/>
+      <c r="E8" s="244"/>
+      <c r="F8" s="244"/>
       <c r="H8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="234"/>
-      <c r="J8" s="235"/>
-      <c r="K8" s="235"/>
-      <c r="L8" s="235"/>
+      <c r="I8" s="241"/>
+      <c r="J8" s="242"/>
+      <c r="K8" s="242"/>
+      <c r="L8" s="242"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="12"/>
-      <c r="C9" s="234"/>
-      <c r="D9" s="234"/>
-      <c r="E9" s="234"/>
-      <c r="F9" s="234"/>
+      <c r="C9" s="241"/>
+      <c r="D9" s="241"/>
+      <c r="E9" s="241"/>
+      <c r="F9" s="241"/>
       <c r="H9" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="234"/>
-      <c r="J9" s="235"/>
-      <c r="K9" s="235"/>
-      <c r="L9" s="235"/>
+      <c r="I9" s="241"/>
+      <c r="J9" s="242"/>
+      <c r="K9" s="242"/>
+      <c r="L9" s="242"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>65</v>
       </c>
       <c r="B10" s="12"/>
-      <c r="C10" s="234"/>
-      <c r="D10" s="234"/>
-      <c r="E10" s="234"/>
-      <c r="F10" s="234"/>
+      <c r="C10" s="241"/>
+      <c r="D10" s="241"/>
+      <c r="E10" s="241"/>
+      <c r="F10" s="241"/>
       <c r="H10" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="234"/>
-      <c r="J10" s="235"/>
-      <c r="K10" s="235"/>
-      <c r="L10" s="235"/>
+      <c r="I10" s="241"/>
+      <c r="J10" s="242"/>
+      <c r="K10" s="242"/>
+      <c r="L10" s="242"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="234"/>
-      <c r="J11" s="235"/>
-      <c r="K11" s="235"/>
-      <c r="L11" s="235"/>
+      <c r="I11" s="241"/>
+      <c r="J11" s="242"/>
+      <c r="K11" s="242"/>
+      <c r="L11" s="242"/>
     </row>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="14"/>
       <c r="H12" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="234"/>
-      <c r="J12" s="235"/>
-      <c r="K12" s="235"/>
-      <c r="L12" s="235"/>
+      <c r="I12" s="241"/>
+      <c r="J12" s="242"/>
+      <c r="K12" s="242"/>
+      <c r="L12" s="242"/>
     </row>
     <row r="13" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H13" s="3"/>
@@ -5469,12 +5473,12 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="244"/>
-      <c r="B16" s="245" t="s">
+      <c r="A16" s="234"/>
+      <c r="B16" s="235" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="238"/>
-      <c r="D16" s="238"/>
+      <c r="C16" s="236"/>
+      <c r="D16" s="236"/>
       <c r="E16" s="18"/>
       <c r="F16" s="128"/>
       <c r="G16" s="128"/>
@@ -5488,12 +5492,12 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="244"/>
+      <c r="A17" s="234"/>
       <c r="B17" s="237" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="238"/>
-      <c r="D17" s="238"/>
+      <c r="C17" s="236"/>
+      <c r="D17" s="236"/>
       <c r="E17" s="18"/>
       <c r="F17" s="128"/>
       <c r="G17" s="128"/>
@@ -5510,8 +5514,8 @@
       <c r="B18" s="237" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="238"/>
-      <c r="D18" s="238"/>
+      <c r="C18" s="236"/>
+      <c r="D18" s="236"/>
       <c r="E18" s="18"/>
       <c r="F18" s="128"/>
       <c r="G18" s="128"/>
@@ -5528,8 +5532,8 @@
       <c r="B19" s="251" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="238"/>
-      <c r="D19" s="238"/>
+      <c r="C19" s="236"/>
+      <c r="D19" s="236"/>
       <c r="E19" s="18"/>
       <c r="F19" s="128"/>
       <c r="G19" s="128"/>
@@ -5546,8 +5550,8 @@
       <c r="B20" s="237" t="s">
         <v>113</v>
       </c>
-      <c r="C20" s="238"/>
-      <c r="D20" s="238"/>
+      <c r="C20" s="236"/>
+      <c r="D20" s="236"/>
       <c r="E20" s="252"/>
       <c r="F20" s="128"/>
       <c r="G20" s="128"/>
@@ -5564,8 +5568,8 @@
       <c r="B21" s="237" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="238"/>
-      <c r="D21" s="238"/>
+      <c r="C21" s="236"/>
+      <c r="D21" s="236"/>
       <c r="E21" s="18"/>
       <c r="F21" s="128"/>
       <c r="G21" s="128"/>
@@ -5579,12 +5583,12 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="246" t="s">
+      <c r="B22" s="238" t="s">
         <v>114</v>
       </c>
-      <c r="C22" s="247"/>
-      <c r="D22" s="247"/>
-      <c r="E22" s="248"/>
+      <c r="C22" s="239"/>
+      <c r="D22" s="239"/>
+      <c r="E22" s="240"/>
       <c r="F22" s="128"/>
       <c r="G22" s="128"/>
       <c r="H22" s="128"/>
@@ -5737,13 +5741,6 @@
     <row r="66" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="I12:L12"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:E20"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="I8:L8"/>
@@ -5756,6 +5753,13 @@
     <mergeCell ref="I10:L10"/>
     <mergeCell ref="I11:L11"/>
     <mergeCell ref="C9:F9"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:E20"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5843,10 +5847,10 @@
         <v>15</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" s="234"/>
-      <c r="D5" s="234"/>
-      <c r="E5" s="234"/>
-      <c r="F5" s="234"/>
+      <c r="C5" s="241"/>
+      <c r="D5" s="241"/>
+      <c r="E5" s="241"/>
+      <c r="F5" s="241"/>
       <c r="H5" s="9"/>
       <c r="I5" s="13" t="s">
         <v>13</v>
@@ -5860,10 +5864,10 @@
         <v>16</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="234"/>
-      <c r="D6" s="234"/>
-      <c r="E6" s="234"/>
-      <c r="F6" s="234"/>
+      <c r="C6" s="241"/>
+      <c r="D6" s="241"/>
+      <c r="E6" s="241"/>
+      <c r="F6" s="241"/>
       <c r="H6" s="1" t="s">
         <v>18</v>
       </c>
@@ -5880,79 +5884,79 @@
       <c r="H7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="239"/>
-      <c r="J7" s="240"/>
-      <c r="K7" s="240"/>
-      <c r="L7" s="241"/>
+      <c r="I7" s="244"/>
+      <c r="J7" s="245"/>
+      <c r="K7" s="245"/>
+      <c r="L7" s="246"/>
     </row>
     <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="239"/>
-      <c r="D8" s="239"/>
-      <c r="E8" s="239"/>
-      <c r="F8" s="239"/>
+      <c r="C8" s="244"/>
+      <c r="D8" s="244"/>
+      <c r="E8" s="244"/>
+      <c r="F8" s="244"/>
       <c r="H8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="234"/>
-      <c r="J8" s="235"/>
-      <c r="K8" s="235"/>
-      <c r="L8" s="236"/>
+      <c r="I8" s="241"/>
+      <c r="J8" s="242"/>
+      <c r="K8" s="242"/>
+      <c r="L8" s="243"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="12"/>
-      <c r="C9" s="234"/>
-      <c r="D9" s="234"/>
-      <c r="E9" s="234"/>
-      <c r="F9" s="234"/>
+      <c r="C9" s="241"/>
+      <c r="D9" s="241"/>
+      <c r="E9" s="241"/>
+      <c r="F9" s="241"/>
       <c r="H9" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="234"/>
-      <c r="J9" s="235"/>
-      <c r="K9" s="235"/>
-      <c r="L9" s="236"/>
+      <c r="I9" s="241"/>
+      <c r="J9" s="242"/>
+      <c r="K9" s="242"/>
+      <c r="L9" s="243"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>65</v>
       </c>
       <c r="B10" s="12"/>
-      <c r="C10" s="234"/>
-      <c r="D10" s="234"/>
-      <c r="E10" s="234"/>
-      <c r="F10" s="234"/>
+      <c r="C10" s="241"/>
+      <c r="D10" s="241"/>
+      <c r="E10" s="241"/>
+      <c r="F10" s="241"/>
       <c r="H10" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="234"/>
-      <c r="J10" s="235"/>
-      <c r="K10" s="235"/>
-      <c r="L10" s="236"/>
+      <c r="I10" s="241"/>
+      <c r="J10" s="242"/>
+      <c r="K10" s="242"/>
+      <c r="L10" s="243"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="234"/>
-      <c r="J11" s="235"/>
-      <c r="K11" s="235"/>
-      <c r="L11" s="236"/>
+      <c r="I11" s="241"/>
+      <c r="J11" s="242"/>
+      <c r="K11" s="242"/>
+      <c r="L11" s="243"/>
     </row>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H12" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="234"/>
-      <c r="J12" s="235"/>
-      <c r="K12" s="235"/>
-      <c r="L12" s="236"/>
+      <c r="I12" s="241"/>
+      <c r="J12" s="242"/>
+      <c r="K12" s="242"/>
+      <c r="L12" s="243"/>
     </row>
     <row r="13" spans="1:12" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H13" s="3"/>
@@ -6262,8 +6266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView showZeros="0" tabSelected="1" view="pageLayout" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -6329,10 +6333,10 @@
         <v>15</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" s="234"/>
-      <c r="D5" s="234"/>
-      <c r="E5" s="234"/>
-      <c r="F5" s="234"/>
+      <c r="C5" s="241"/>
+      <c r="D5" s="241"/>
+      <c r="E5" s="241"/>
+      <c r="F5" s="241"/>
       <c r="H5" s="9"/>
       <c r="I5" s="13" t="s">
         <v>13</v>
@@ -6346,10 +6350,10 @@
         <v>16</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="234"/>
-      <c r="D6" s="234"/>
-      <c r="E6" s="234"/>
-      <c r="F6" s="234"/>
+      <c r="C6" s="241"/>
+      <c r="D6" s="241"/>
+      <c r="E6" s="241"/>
+      <c r="F6" s="241"/>
       <c r="H6" s="1" t="s">
         <v>18</v>
       </c>
@@ -6366,79 +6370,79 @@
       <c r="H7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="239"/>
-      <c r="J7" s="240"/>
-      <c r="K7" s="240"/>
-      <c r="L7" s="241"/>
+      <c r="I7" s="244"/>
+      <c r="J7" s="245"/>
+      <c r="K7" s="245"/>
+      <c r="L7" s="246"/>
     </row>
     <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="239"/>
-      <c r="D8" s="239"/>
-      <c r="E8" s="239"/>
-      <c r="F8" s="239"/>
+      <c r="C8" s="244"/>
+      <c r="D8" s="244"/>
+      <c r="E8" s="244"/>
+      <c r="F8" s="244"/>
       <c r="H8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="234"/>
-      <c r="J8" s="235"/>
-      <c r="K8" s="235"/>
-      <c r="L8" s="236"/>
+      <c r="I8" s="241"/>
+      <c r="J8" s="242"/>
+      <c r="K8" s="242"/>
+      <c r="L8" s="243"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="12"/>
-      <c r="C9" s="234"/>
-      <c r="D9" s="234"/>
-      <c r="E9" s="234"/>
-      <c r="F9" s="234"/>
+      <c r="C9" s="241"/>
+      <c r="D9" s="241"/>
+      <c r="E9" s="241"/>
+      <c r="F9" s="241"/>
       <c r="H9" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="234"/>
-      <c r="J9" s="235"/>
-      <c r="K9" s="235"/>
-      <c r="L9" s="236"/>
+      <c r="I9" s="241"/>
+      <c r="J9" s="242"/>
+      <c r="K9" s="242"/>
+      <c r="L9" s="243"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>65</v>
       </c>
       <c r="B10" s="12"/>
-      <c r="C10" s="234"/>
-      <c r="D10" s="234"/>
-      <c r="E10" s="234"/>
-      <c r="F10" s="234"/>
+      <c r="C10" s="241"/>
+      <c r="D10" s="241"/>
+      <c r="E10" s="241"/>
+      <c r="F10" s="241"/>
       <c r="H10" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="234"/>
-      <c r="J10" s="235"/>
-      <c r="K10" s="235"/>
-      <c r="L10" s="236"/>
+      <c r="I10" s="241"/>
+      <c r="J10" s="242"/>
+      <c r="K10" s="242"/>
+      <c r="L10" s="243"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="234"/>
-      <c r="J11" s="235"/>
-      <c r="K11" s="235"/>
-      <c r="L11" s="236"/>
+      <c r="I11" s="241"/>
+      <c r="J11" s="242"/>
+      <c r="K11" s="242"/>
+      <c r="L11" s="243"/>
     </row>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H12" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="234"/>
-      <c r="J12" s="235"/>
-      <c r="K12" s="235"/>
-      <c r="L12" s="236"/>
+      <c r="I12" s="241"/>
+      <c r="J12" s="242"/>
+      <c r="K12" s="242"/>
+      <c r="L12" s="243"/>
     </row>
     <row r="13" spans="1:12" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H13" s="3"/>
@@ -6464,13 +6468,32 @@
       <c r="L14" s="55"/>
     </row>
     <row r="15" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="25"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="56"/>
+      <c r="A15" s="267"/>
+      <c r="B15" s="269"/>
+      <c r="C15" s="269"/>
+      <c r="D15" s="269"/>
+      <c r="E15" s="269"/>
+      <c r="F15" s="269"/>
+      <c r="G15" s="269"/>
+      <c r="H15" s="269"/>
+      <c r="I15" s="269"/>
+      <c r="J15" s="269"/>
+      <c r="K15" s="269"/>
+      <c r="L15" s="270"/>
     </row>
     <row r="16" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="25"/>
-      <c r="L16" s="26"/>
+      <c r="A16" s="268"/>
+      <c r="B16" s="245"/>
+      <c r="C16" s="245"/>
+      <c r="D16" s="245"/>
+      <c r="E16" s="245"/>
+      <c r="F16" s="245"/>
+      <c r="G16" s="245"/>
+      <c r="H16" s="245"/>
+      <c r="I16" s="245"/>
+      <c r="J16" s="245"/>
+      <c r="K16" s="245"/>
+      <c r="L16" s="246"/>
     </row>
     <row r="17" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="108" t="s">
@@ -6509,7 +6532,10 @@
       </c>
       <c r="C20" s="47"/>
       <c r="D20" s="62"/>
-      <c r="E20" s="129"/>
+      <c r="E20" s="129">
+        <f>LEN(A$15)-LEN(SUBSTITUTE(A$15,"D",""))+LEN(A$15)-LEN(SUBSTITUTE(A$15,"S",""))</f>
+        <v>0</v>
+      </c>
       <c r="F20" s="90">
         <v>0.5</v>
       </c>
@@ -6528,7 +6554,10 @@
       </c>
       <c r="C21" s="47"/>
       <c r="D21" s="62"/>
-      <c r="E21" s="129"/>
+      <c r="E21" s="129">
+        <f>LEN(A$15)-LEN(SUBSTITUTE(A$15,"M",""))</f>
+        <v>0</v>
+      </c>
       <c r="F21" s="90">
         <v>0.3</v>
       </c>
@@ -6547,7 +6576,10 @@
       </c>
       <c r="C22" s="47"/>
       <c r="D22" s="62"/>
-      <c r="E22" s="129"/>
+      <c r="E22" s="129">
+        <f>LEN(A$15)-LEN(SUBSTITUTE(A$15,"E",""))+LEN(A$15)-LEN(SUBSTITUTE(A$15,"L",""))</f>
+        <v>0</v>
+      </c>
       <c r="F22" s="90">
         <v>0.1</v>
       </c>
@@ -6615,7 +6647,11 @@
       </c>
       <c r="C27" s="48"/>
       <c r="D27" s="62"/>
-      <c r="E27" s="129"/>
+      <c r="E27" s="129">
+        <f xml:space="preserve">
+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"1","")))*1+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"2","")))*2+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"3","")))*3+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"4","")))*4+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"5","")))*5+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"6","")))*6+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"7","")))*7+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"8","")))*8+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"9","")))*9</f>
+        <v>0</v>
+      </c>
       <c r="F27" s="47" t="s">
         <v>51</v>
       </c>
@@ -6719,7 +6755,8 @@
       <c r="L42" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="A15:L16"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="I7:L7"/>
     <mergeCell ref="I8:L8"/>
@@ -6749,7 +6786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" view="pageLayout" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -6816,10 +6853,10 @@
         <v>15</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" s="234"/>
-      <c r="D5" s="234"/>
-      <c r="E5" s="234"/>
-      <c r="F5" s="234"/>
+      <c r="C5" s="241"/>
+      <c r="D5" s="241"/>
+      <c r="E5" s="241"/>
+      <c r="F5" s="241"/>
       <c r="H5" s="9"/>
       <c r="I5" s="13" t="s">
         <v>13</v>
@@ -6833,10 +6870,10 @@
         <v>16</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="234"/>
-      <c r="D6" s="234"/>
-      <c r="E6" s="234"/>
-      <c r="F6" s="234"/>
+      <c r="C6" s="241"/>
+      <c r="D6" s="241"/>
+      <c r="E6" s="241"/>
+      <c r="F6" s="241"/>
       <c r="H6" s="1" t="s">
         <v>18</v>
       </c>
@@ -6853,79 +6890,79 @@
       <c r="H7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="239"/>
-      <c r="J7" s="240"/>
-      <c r="K7" s="240"/>
-      <c r="L7" s="241"/>
+      <c r="I7" s="244"/>
+      <c r="J7" s="245"/>
+      <c r="K7" s="245"/>
+      <c r="L7" s="246"/>
     </row>
     <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="239"/>
-      <c r="D8" s="239"/>
-      <c r="E8" s="239"/>
-      <c r="F8" s="239"/>
+      <c r="C8" s="244"/>
+      <c r="D8" s="244"/>
+      <c r="E8" s="244"/>
+      <c r="F8" s="244"/>
       <c r="H8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="234"/>
-      <c r="J8" s="235"/>
-      <c r="K8" s="235"/>
-      <c r="L8" s="236"/>
+      <c r="I8" s="241"/>
+      <c r="J8" s="242"/>
+      <c r="K8" s="242"/>
+      <c r="L8" s="243"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="12"/>
-      <c r="C9" s="234"/>
-      <c r="D9" s="234"/>
-      <c r="E9" s="234"/>
-      <c r="F9" s="234"/>
+      <c r="C9" s="241"/>
+      <c r="D9" s="241"/>
+      <c r="E9" s="241"/>
+      <c r="F9" s="241"/>
       <c r="H9" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="234"/>
-      <c r="J9" s="235"/>
-      <c r="K9" s="235"/>
-      <c r="L9" s="236"/>
+      <c r="I9" s="241"/>
+      <c r="J9" s="242"/>
+      <c r="K9" s="242"/>
+      <c r="L9" s="243"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>65</v>
       </c>
       <c r="B10" s="12"/>
-      <c r="C10" s="234"/>
-      <c r="D10" s="234"/>
-      <c r="E10" s="234"/>
-      <c r="F10" s="234"/>
+      <c r="C10" s="241"/>
+      <c r="D10" s="241"/>
+      <c r="E10" s="241"/>
+      <c r="F10" s="241"/>
       <c r="H10" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="234"/>
-      <c r="J10" s="235"/>
-      <c r="K10" s="235"/>
-      <c r="L10" s="236"/>
+      <c r="I10" s="241"/>
+      <c r="J10" s="242"/>
+      <c r="K10" s="242"/>
+      <c r="L10" s="243"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="234"/>
-      <c r="J11" s="235"/>
-      <c r="K11" s="235"/>
-      <c r="L11" s="236"/>
+      <c r="I11" s="241"/>
+      <c r="J11" s="242"/>
+      <c r="K11" s="242"/>
+      <c r="L11" s="243"/>
     </row>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H12" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="234"/>
-      <c r="J12" s="235"/>
-      <c r="K12" s="235"/>
-      <c r="L12" s="236"/>
+      <c r="I12" s="241"/>
+      <c r="J12" s="242"/>
+      <c r="K12" s="242"/>
+      <c r="L12" s="243"/>
     </row>
     <row r="13" spans="1:12" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H13" s="3"/>
@@ -6951,13 +6988,32 @@
       <c r="L14" s="55"/>
     </row>
     <row r="15" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="25"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="56"/>
+      <c r="A15" s="267"/>
+      <c r="B15" s="269"/>
+      <c r="C15" s="269"/>
+      <c r="D15" s="269"/>
+      <c r="E15" s="269"/>
+      <c r="F15" s="269"/>
+      <c r="G15" s="269"/>
+      <c r="H15" s="269"/>
+      <c r="I15" s="269"/>
+      <c r="J15" s="269"/>
+      <c r="K15" s="269"/>
+      <c r="L15" s="270"/>
     </row>
     <row r="16" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="25"/>
-      <c r="L16" s="26"/>
+      <c r="A16" s="268"/>
+      <c r="B16" s="245"/>
+      <c r="C16" s="245"/>
+      <c r="D16" s="245"/>
+      <c r="E16" s="245"/>
+      <c r="F16" s="245"/>
+      <c r="G16" s="245"/>
+      <c r="H16" s="245"/>
+      <c r="I16" s="245"/>
+      <c r="J16" s="245"/>
+      <c r="K16" s="245"/>
+      <c r="L16" s="246"/>
     </row>
     <row r="17" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="108" t="s">
@@ -6997,6 +7053,7 @@
       <c r="C20" s="47"/>
       <c r="D20" s="62"/>
       <c r="E20" s="129">
+        <f>LEN(A$15)-LEN(SUBSTITUTE(A$15,"D",""))+LEN(A$15)-LEN(SUBSTITUTE(A$15,"S",""))</f>
         <v>0</v>
       </c>
       <c r="F20" s="90">
@@ -7022,6 +7079,7 @@
       <c r="C21" s="47"/>
       <c r="D21" s="62"/>
       <c r="E21" s="129">
+        <f>LEN(A$15)-LEN(SUBSTITUTE(A$15,"M",""))</f>
         <v>0</v>
       </c>
       <c r="F21" s="90">
@@ -7047,6 +7105,7 @@
       <c r="C22" s="47"/>
       <c r="D22" s="62"/>
       <c r="E22" s="129">
+        <f>LEN(A$15)-LEN(SUBSTITUTE(A$15,"E",""))+LEN(A$15)-LEN(SUBSTITUTE(A$15,"L",""))</f>
         <v>0</v>
       </c>
       <c r="F22" s="90">
@@ -7140,6 +7199,8 @@
       <c r="C28" s="48"/>
       <c r="D28" s="62"/>
       <c r="E28" s="129">
+        <f xml:space="preserve">
+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"1","")))*1+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"2","")))*2+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"3","")))*3+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"4","")))*4+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"5","")))*5+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"6","")))*6+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"7","")))*7+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"8","")))*8+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$15,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"9","")))*9</f>
         <v>0</v>
       </c>
       <c r="F28" s="47" t="s">
@@ -7238,7 +7299,8 @@
       <c r="L42" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="A15:L16"/>
     <mergeCell ref="I12:L12"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="I7:L7"/>
@@ -7267,8 +7329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" view="pageLayout" topLeftCell="B10" zoomScale="110" zoomScaleNormal="120" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView showZeros="0" view="pageLayout" topLeftCell="A10" zoomScale="110" zoomScaleNormal="120" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -7334,10 +7396,10 @@
         <v>15</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" s="234"/>
-      <c r="D5" s="234"/>
-      <c r="E5" s="234"/>
-      <c r="F5" s="234"/>
+      <c r="C5" s="241"/>
+      <c r="D5" s="241"/>
+      <c r="E5" s="241"/>
+      <c r="F5" s="241"/>
       <c r="H5" s="9"/>
       <c r="I5" s="13" t="s">
         <v>13</v>
@@ -7351,10 +7413,10 @@
         <v>16</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="234"/>
-      <c r="D6" s="234"/>
-      <c r="E6" s="234"/>
-      <c r="F6" s="234"/>
+      <c r="C6" s="241"/>
+      <c r="D6" s="241"/>
+      <c r="E6" s="241"/>
+      <c r="F6" s="241"/>
       <c r="H6" s="1" t="s">
         <v>18</v>
       </c>
@@ -7371,80 +7433,80 @@
       <c r="H7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="239"/>
-      <c r="J7" s="240"/>
-      <c r="K7" s="240"/>
-      <c r="L7" s="241"/>
+      <c r="I7" s="244"/>
+      <c r="J7" s="245"/>
+      <c r="K7" s="245"/>
+      <c r="L7" s="246"/>
     </row>
     <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="239"/>
-      <c r="D8" s="239"/>
-      <c r="E8" s="239"/>
-      <c r="F8" s="239"/>
+      <c r="C8" s="244"/>
+      <c r="D8" s="244"/>
+      <c r="E8" s="244"/>
+      <c r="F8" s="244"/>
       <c r="H8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="234"/>
-      <c r="J8" s="235"/>
-      <c r="K8" s="235"/>
-      <c r="L8" s="236"/>
+      <c r="I8" s="241"/>
+      <c r="J8" s="242"/>
+      <c r="K8" s="242"/>
+      <c r="L8" s="243"/>
     </row>
     <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="12"/>
-      <c r="C9" s="234"/>
-      <c r="D9" s="234"/>
-      <c r="E9" s="234"/>
-      <c r="F9" s="234"/>
+      <c r="C9" s="241"/>
+      <c r="D9" s="241"/>
+      <c r="E9" s="241"/>
+      <c r="F9" s="241"/>
       <c r="H9" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="234"/>
-      <c r="J9" s="235"/>
-      <c r="K9" s="235"/>
-      <c r="L9" s="236"/>
+      <c r="I9" s="241"/>
+      <c r="J9" s="242"/>
+      <c r="K9" s="242"/>
+      <c r="L9" s="243"/>
     </row>
     <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>65</v>
       </c>
       <c r="B10" s="12"/>
-      <c r="C10" s="234"/>
-      <c r="D10" s="234"/>
-      <c r="E10" s="234"/>
-      <c r="F10" s="234"/>
+      <c r="C10" s="241"/>
+      <c r="D10" s="241"/>
+      <c r="E10" s="241"/>
+      <c r="F10" s="241"/>
       <c r="H10" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="234"/>
-      <c r="J10" s="235"/>
-      <c r="K10" s="235"/>
-      <c r="L10" s="236"/>
+      <c r="I10" s="241"/>
+      <c r="J10" s="242"/>
+      <c r="K10" s="242"/>
+      <c r="L10" s="243"/>
     </row>
     <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="234"/>
-      <c r="J11" s="235"/>
-      <c r="K11" s="235"/>
-      <c r="L11" s="236"/>
+      <c r="I11" s="241"/>
+      <c r="J11" s="242"/>
+      <c r="K11" s="242"/>
+      <c r="L11" s="243"/>
     </row>
     <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="14"/>
       <c r="H12" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="234"/>
-      <c r="J12" s="235"/>
-      <c r="K12" s="235"/>
-      <c r="L12" s="236"/>
+      <c r="I12" s="241"/>
+      <c r="J12" s="242"/>
+      <c r="K12" s="242"/>
+      <c r="L12" s="243"/>
     </row>
     <row r="13" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="14"/>
@@ -7463,16 +7525,16 @@
       <c r="A15" s="253" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="255" t="s">
+      <c r="B15" s="257" t="s">
         <v>108</v>
       </c>
-      <c r="C15" s="256"/>
-      <c r="D15" s="256"/>
-      <c r="E15" s="256"/>
-      <c r="F15" s="256"/>
-      <c r="G15" s="256"/>
-      <c r="H15" s="256"/>
-      <c r="I15" s="257"/>
+      <c r="C15" s="258"/>
+      <c r="D15" s="258"/>
+      <c r="E15" s="258"/>
+      <c r="F15" s="258"/>
+      <c r="G15" s="258"/>
+      <c r="H15" s="258"/>
+      <c r="I15" s="259"/>
       <c r="J15" s="79" t="s">
         <v>7</v>
       </c>
@@ -7485,16 +7547,16 @@
     </row>
     <row r="16" spans="1:13" ht="83.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="254"/>
-      <c r="B16" s="258" t="s">
+      <c r="B16" s="260" t="s">
         <v>109</v>
       </c>
-      <c r="C16" s="259"/>
-      <c r="D16" s="259"/>
-      <c r="E16" s="259"/>
-      <c r="F16" s="259"/>
-      <c r="G16" s="259"/>
-      <c r="H16" s="259"/>
-      <c r="I16" s="259"/>
+      <c r="C16" s="261"/>
+      <c r="D16" s="261"/>
+      <c r="E16" s="261"/>
+      <c r="F16" s="261"/>
+      <c r="G16" s="261"/>
+      <c r="H16" s="261"/>
+      <c r="I16" s="261"/>
       <c r="J16" s="82" t="s">
         <v>8</v>
       </c>
@@ -7506,7 +7568,7 @@
       <c r="M16" s="81"/>
     </row>
     <row r="17" spans="1:13" ht="115.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="265" t="s">
+      <c r="A17" s="255" t="s">
         <v>62</v>
       </c>
       <c r="B17" s="262" t="s">
@@ -7530,17 +7592,17 @@
       <c r="M17" s="81"/>
     </row>
     <row r="18" spans="1:13" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="266"/>
-      <c r="B18" s="260" t="s">
+      <c r="A18" s="256"/>
+      <c r="B18" s="265" t="s">
         <v>112</v>
       </c>
-      <c r="C18" s="261"/>
-      <c r="D18" s="261"/>
-      <c r="E18" s="261"/>
-      <c r="F18" s="261"/>
-      <c r="G18" s="261"/>
-      <c r="H18" s="261"/>
-      <c r="I18" s="261"/>
+      <c r="C18" s="266"/>
+      <c r="D18" s="266"/>
+      <c r="E18" s="266"/>
+      <c r="F18" s="266"/>
+      <c r="G18" s="266"/>
+      <c r="H18" s="266"/>
+      <c r="I18" s="266"/>
       <c r="J18" s="85" t="s">
         <v>9</v>
       </c>
@@ -7581,7 +7643,7 @@
     <row r="22" spans="1:13" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="L22" s="69"/>
     </row>
-    <row r="23" spans="1:13" ht="13.9" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I23" s="50" t="s">
         <v>64</v>
       </c>
@@ -7610,12 +7672,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B15:I15"/>
-    <mergeCell ref="B16:I16"/>
-    <mergeCell ref="B17:I17"/>
-    <mergeCell ref="B18:I18"/>
     <mergeCell ref="I12:L12"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="I7:L7"/>
@@ -7627,6 +7683,12 @@
     <mergeCell ref="I10:L10"/>
     <mergeCell ref="I11:L11"/>
     <mergeCell ref="C6:F6"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B15:I15"/>
+    <mergeCell ref="B16:I16"/>
+    <mergeCell ref="B17:I17"/>
+    <mergeCell ref="B18:I18"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7641,24 +7703,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100570C130F412EDB4EBF3E80DF6A9149FD" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfaa3b10b9be17ef9f56bd19dc71004c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddb0c952b897a810c8a4e377cff6bff8" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -7724,10 +7768,37 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A00BD0D-8423-4FFE-92A4-D273D2078383}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7748,18 +7819,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A00BD0D-8423-4FFE-92A4-D273D2078383}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Protokoll olika % för junior och seniorlag art
</commit_message>
<xml_diff>
--- a/mallar/Protokoll/Protokoll_2019_lag_sv-r_mellan(mall).xlsx
+++ b/mallar/Protokoll/Protokoll_2019_lag_sv-r_mellan(mall).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\episerver\voltige\VoltigeClosedXML\mallar\Protokoll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FE158A-834D-4AB9-8AAB-46D79CAEDA31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54E0CEE-B78A-46E4-8FB4-DD51AEAB4E7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43080" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="27" r:id="rId1"/>
@@ -22,10 +22,11 @@
     <sheet name="Lag kür tekn junior" sheetId="6" r:id="rId7"/>
     <sheet name="Lag kür tekn sr" sheetId="20" r:id="rId8"/>
     <sheet name="Lag kür art" sheetId="21" r:id="rId9"/>
+    <sheet name="Lag kür art senior" sheetId="31" r:id="rId10"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId10"/>
     <externalReference r:id="rId11"/>
+    <externalReference r:id="rId12"/>
   </externalReferences>
   <definedNames>
     <definedName name="Antal_tävlingsdagar" localSheetId="1">[1]Information!$H$5</definedName>
@@ -35,6 +36,7 @@
     <definedName name="bord" localSheetId="4">'Lag grund B'!$L$3</definedName>
     <definedName name="bord" localSheetId="3">'Lag grund D'!$L$3</definedName>
     <definedName name="bord" localSheetId="8">'Lag kür art'!$L$3</definedName>
+    <definedName name="bord" localSheetId="9">'Lag kür art senior'!$L$3</definedName>
     <definedName name="bord" localSheetId="6">'Lag kür tekn junior'!$L$3</definedName>
     <definedName name="bord" localSheetId="5">'Lag kür tekn mellan'!$L$3</definedName>
     <definedName name="bord" localSheetId="7">'Lag kür tekn sr'!$L$3</definedName>
@@ -43,6 +45,7 @@
     <definedName name="datum" localSheetId="4">'Lag grund B'!$C$4</definedName>
     <definedName name="datum" localSheetId="3">'Lag grund D'!$C$4</definedName>
     <definedName name="datum" localSheetId="8">'Lag kür art'!$C$4</definedName>
+    <definedName name="datum" localSheetId="9">'Lag kür art senior'!$C$4</definedName>
     <definedName name="datum" localSheetId="6">'Lag kür tekn junior'!$C$4</definedName>
     <definedName name="datum" localSheetId="5">'Lag kür tekn mellan'!$C$4</definedName>
     <definedName name="datum" localSheetId="7">'Lag kür tekn sr'!$C$4</definedName>
@@ -51,6 +54,7 @@
     <definedName name="domare" localSheetId="4">'Lag grund B'!$C$32</definedName>
     <definedName name="domare" localSheetId="3">'Lag grund D'!$C$33</definedName>
     <definedName name="domare" localSheetId="8">'Lag kür art'!$C$27</definedName>
+    <definedName name="domare" localSheetId="9">'Lag kür art senior'!$C$27</definedName>
     <definedName name="domare" localSheetId="6">'Lag kür tekn junior'!$C$42</definedName>
     <definedName name="domare" localSheetId="5">'Lag kür tekn mellan'!$C$42</definedName>
     <definedName name="domare" localSheetId="7">'Lag kür tekn sr'!$C$42</definedName>
@@ -59,6 +63,7 @@
     <definedName name="firstvaulter" localSheetId="4">'Lag grund B'!$I$7</definedName>
     <definedName name="firstvaulter" localSheetId="3">'Lag grund D'!$I$7</definedName>
     <definedName name="firstvaulter" localSheetId="8">'Lag kür art'!$I$7</definedName>
+    <definedName name="firstvaulter" localSheetId="9">'Lag kür art senior'!$I$7</definedName>
     <definedName name="firstvaulter" localSheetId="6">'Lag kür tekn junior'!$I$7</definedName>
     <definedName name="firstvaulter" localSheetId="5">'Lag kür tekn mellan'!$I$7</definedName>
     <definedName name="firstvaulter" localSheetId="7">'Lag kür tekn sr'!$I$7</definedName>
@@ -68,6 +73,7 @@
     <definedName name="id" localSheetId="4">'Lag grund B'!$U$1</definedName>
     <definedName name="id" localSheetId="3">'Lag grund D'!$U$1</definedName>
     <definedName name="id" localSheetId="8">'Lag kür art'!$U$1</definedName>
+    <definedName name="id" localSheetId="9">'Lag kür art senior'!$U$1</definedName>
     <definedName name="id" localSheetId="6">'Lag kür tekn junior'!$U$1</definedName>
     <definedName name="id" localSheetId="5">'Lag kür tekn mellan'!$U$1</definedName>
     <definedName name="id" localSheetId="7">'Lag kür tekn sr'!$U$1</definedName>
@@ -76,6 +82,7 @@
     <definedName name="klass" localSheetId="4">'Lag grund B'!$L$4</definedName>
     <definedName name="klass" localSheetId="3">'Lag grund D'!$L$4</definedName>
     <definedName name="klass" localSheetId="8">'Lag kür art'!$L$4</definedName>
+    <definedName name="klass" localSheetId="9">'Lag kür art senior'!$L$4</definedName>
     <definedName name="klass" localSheetId="6">'Lag kür tekn junior'!$L$4</definedName>
     <definedName name="klass" localSheetId="5">'Lag kür tekn mellan'!$L$4</definedName>
     <definedName name="klass" localSheetId="7">'Lag kür tekn sr'!$L$4</definedName>
@@ -84,6 +91,7 @@
     <definedName name="moment" localSheetId="4">'Lag grund B'!$L$5</definedName>
     <definedName name="moment" localSheetId="3">'Lag grund D'!$L$5</definedName>
     <definedName name="moment" localSheetId="8">'Lag kür art'!$L$5</definedName>
+    <definedName name="moment" localSheetId="9">'Lag kür art senior'!$L$5</definedName>
     <definedName name="moment" localSheetId="6">'Lag kür tekn junior'!$L$5</definedName>
     <definedName name="moment" localSheetId="5">'Lag kür tekn mellan'!$L$5</definedName>
     <definedName name="moment" localSheetId="7">'Lag kür tekn sr'!$L$5</definedName>
@@ -92,6 +100,7 @@
     <definedName name="result" localSheetId="4">'Lag grund B'!$L$29</definedName>
     <definedName name="result" localSheetId="3">'Lag grund D'!$L$29</definedName>
     <definedName name="result" localSheetId="8">'Lag kür art'!$L$24</definedName>
+    <definedName name="result" localSheetId="9">'Lag kür art senior'!$L$24</definedName>
     <definedName name="result" localSheetId="6">'Lag kür tekn junior'!$L$34</definedName>
     <definedName name="result" localSheetId="5">'Lag kür tekn mellan'!$L$34</definedName>
     <definedName name="result" localSheetId="7">'Lag kür tekn sr'!$L$35</definedName>
@@ -112,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="149">
   <si>
     <t>1)</t>
   </si>
@@ -868,6 +877,21 @@
   </si>
   <si>
     <t>KOREOGRAFI</t>
+  </si>
+  <si>
+    <t>C1
+20%</t>
+  </si>
+  <si>
+    <t>C3
+25%</t>
+  </si>
+  <si>
+    <t>C4
+25%</t>
+  </si>
+  <si>
+    <t>Lag kür senior</t>
   </si>
 </sst>
 </file>
@@ -2304,6 +2328,239 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="9" fontId="25" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="25" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="60" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="52" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="43" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="61" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="62" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="53" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="53" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="48" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="53" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="57" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="58" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="25" fillId="0" borderId="59" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="55" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="42" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -2322,265 +2579,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="42" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="53" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="48" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="53" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="57" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="58" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="25" fillId="0" borderId="59" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="55" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="9" fontId="25" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="25" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="60" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="52" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="43" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="61" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="62" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="53" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2592,6 +2601,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
@@ -2622,6 +2646,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -2656,15 +2689,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3895,6 +3919,418 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76E92013-7EE9-4BBB-985C-F7F686664514}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:M28"/>
+  <sheetViews>
+    <sheetView showZeros="0" tabSelected="1" view="pageLayout" zoomScale="110" zoomScaleNormal="120" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" style="1"/>
+    <col min="3" max="3" width="12.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.73046875" style="1" customWidth="1"/>
+    <col min="5" max="7" width="7.265625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.265625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="4.73046875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.265625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.73046875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="7.265625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.1328125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="H2" s="9"/>
+      <c r="I2" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" s="10"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+    </row>
+    <row r="3" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="9"/>
+      <c r="I3" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J3" s="10"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+    </row>
+    <row r="4" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="126"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="J4" s="10"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="135"/>
+    </row>
+    <row r="5" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="261"/>
+      <c r="D5" s="261"/>
+      <c r="E5" s="261"/>
+      <c r="F5" s="261"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="106"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+    </row>
+    <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="261"/>
+      <c r="D6" s="261"/>
+      <c r="E6" s="261"/>
+      <c r="F6" s="261"/>
+      <c r="H6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="H7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7" s="266"/>
+      <c r="J7" s="267"/>
+      <c r="K7" s="267"/>
+      <c r="L7" s="268"/>
+    </row>
+    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="266"/>
+      <c r="D8" s="266"/>
+      <c r="E8" s="266"/>
+      <c r="F8" s="266"/>
+      <c r="H8" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="261"/>
+      <c r="J8" s="262"/>
+      <c r="K8" s="262"/>
+      <c r="L8" s="263"/>
+    </row>
+    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="261"/>
+      <c r="D9" s="261"/>
+      <c r="E9" s="261"/>
+      <c r="F9" s="261"/>
+      <c r="H9" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9" s="261"/>
+      <c r="J9" s="262"/>
+      <c r="K9" s="262"/>
+      <c r="L9" s="263"/>
+    </row>
+    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="261"/>
+      <c r="D10" s="261"/>
+      <c r="E10" s="261"/>
+      <c r="F10" s="261"/>
+      <c r="H10" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" s="261"/>
+      <c r="J10" s="262"/>
+      <c r="K10" s="262"/>
+      <c r="L10" s="263"/>
+    </row>
+    <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H11" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="261"/>
+      <c r="J11" s="262"/>
+      <c r="K11" s="262"/>
+      <c r="L11" s="263"/>
+    </row>
+    <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="14"/>
+      <c r="H12" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" s="261"/>
+      <c r="J12" s="262"/>
+      <c r="K12" s="262"/>
+      <c r="L12" s="263"/>
+    </row>
+    <row r="13" spans="1:13" ht="8.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="14"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:13" ht="20.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="14"/>
+      <c r="I14" s="66"/>
+      <c r="K14" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="172" t="s">
+        <v>127</v>
+      </c>
+      <c r="B15" s="288" t="s">
+        <v>128</v>
+      </c>
+      <c r="C15" s="289"/>
+      <c r="D15" s="289"/>
+      <c r="E15" s="289"/>
+      <c r="F15" s="289"/>
+      <c r="G15" s="289"/>
+      <c r="H15" s="289"/>
+      <c r="I15" s="290"/>
+      <c r="J15" s="173" t="s">
+        <v>129</v>
+      </c>
+      <c r="K15" s="174"/>
+      <c r="L15" s="175">
+        <f>K15*0.2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="66.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="291" t="s">
+        <v>143</v>
+      </c>
+      <c r="B16" s="295" t="s">
+        <v>141</v>
+      </c>
+      <c r="C16" s="296"/>
+      <c r="D16" s="296"/>
+      <c r="E16" s="296"/>
+      <c r="F16" s="296"/>
+      <c r="G16" s="296"/>
+      <c r="H16" s="296"/>
+      <c r="I16" s="296"/>
+      <c r="J16" s="78" t="s">
+        <v>138</v>
+      </c>
+      <c r="K16" s="130"/>
+      <c r="L16" s="79">
+        <f>K16*0.1</f>
+        <v>0</v>
+      </c>
+      <c r="M16" s="80"/>
+    </row>
+    <row r="17" spans="1:13" ht="83.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="292"/>
+      <c r="B17" s="295" t="s">
+        <v>142</v>
+      </c>
+      <c r="C17" s="296"/>
+      <c r="D17" s="296"/>
+      <c r="E17" s="296"/>
+      <c r="F17" s="296"/>
+      <c r="G17" s="296"/>
+      <c r="H17" s="296"/>
+      <c r="I17" s="296"/>
+      <c r="J17" s="81" t="s">
+        <v>130</v>
+      </c>
+      <c r="K17" s="131"/>
+      <c r="L17" s="82">
+        <f>K17*0.1</f>
+        <v>0</v>
+      </c>
+      <c r="M17" s="80"/>
+    </row>
+    <row r="18" spans="1:13" ht="58.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="293" t="s">
+        <v>144</v>
+      </c>
+      <c r="B18" s="297" t="s">
+        <v>131</v>
+      </c>
+      <c r="C18" s="298"/>
+      <c r="D18" s="298"/>
+      <c r="E18" s="298"/>
+      <c r="F18" s="298"/>
+      <c r="G18" s="298"/>
+      <c r="H18" s="298"/>
+      <c r="I18" s="299"/>
+      <c r="J18" s="78" t="s">
+        <v>139</v>
+      </c>
+      <c r="K18" s="132"/>
+      <c r="L18" s="83">
+        <f>K18*0.3</f>
+        <v>0</v>
+      </c>
+      <c r="M18" s="80"/>
+    </row>
+    <row r="19" spans="1:13" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="294"/>
+      <c r="B19" s="300" t="s">
+        <v>132</v>
+      </c>
+      <c r="C19" s="301"/>
+      <c r="D19" s="301"/>
+      <c r="E19" s="301"/>
+      <c r="F19" s="301"/>
+      <c r="G19" s="301"/>
+      <c r="H19" s="301"/>
+      <c r="I19" s="302"/>
+      <c r="J19" s="84" t="s">
+        <v>140</v>
+      </c>
+      <c r="K19" s="133"/>
+      <c r="L19" s="85">
+        <f>K19*0.3</f>
+        <v>0</v>
+      </c>
+      <c r="M19" s="80"/>
+    </row>
+    <row r="20" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L20" s="86">
+        <f>SUM(L16:L19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L21" s="68"/>
+    </row>
+    <row r="22" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="61"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="48"/>
+      <c r="K22" s="48"/>
+      <c r="L22" s="134"/>
+    </row>
+    <row r="23" spans="1:13" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L23" s="68"/>
+    </row>
+    <row r="24" spans="1:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I24" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="J24" s="76"/>
+      <c r="K24" s="76"/>
+      <c r="L24" s="77">
+        <f>SUM(L15:L19)-L22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="8.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="H27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B28" s="66"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="66"/>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="I11:L11"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="B15:I15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:I16"/>
+    <mergeCell ref="B17:I17"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="I9:L9"/>
+  </mergeCells>
+  <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;L&amp;G
+&amp;C&amp;"Verdana,Normal"&amp;12PROTOKOLL FÖR LAGTÄVLAN</oddHeader>
+    <oddFooter>&amp;R&amp;8 2025-03-16</oddFooter>
+  </headerFooter>
+  <legacyDrawingHF r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C25329-D17D-4FF2-BF65-A450782F317F}">
   <sheetPr>
@@ -3902,7 +4338,7 @@
   </sheetPr>
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" view="pageLayout" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -3951,8 +4387,8 @@
         <v>11</v>
       </c>
       <c r="B4" s="146"/>
-      <c r="C4" s="183"/>
-      <c r="D4" s="183"/>
+      <c r="C4" s="258"/>
+      <c r="D4" s="258"/>
       <c r="E4" s="147"/>
       <c r="G4" s="140"/>
       <c r="H4" s="141" t="s">
@@ -3967,9 +4403,9 @@
         <v>12</v>
       </c>
       <c r="B5" s="148"/>
-      <c r="C5" s="181"/>
-      <c r="D5" s="181"/>
-      <c r="E5" s="181"/>
+      <c r="C5" s="256"/>
+      <c r="D5" s="256"/>
+      <c r="E5" s="256"/>
       <c r="G5" s="140"/>
       <c r="H5" s="141" t="s">
         <v>10</v>
@@ -3983,9 +4419,9 @@
         <v>13</v>
       </c>
       <c r="B6" s="148"/>
-      <c r="C6" s="181"/>
-      <c r="D6" s="181"/>
-      <c r="E6" s="181"/>
+      <c r="C6" s="256"/>
+      <c r="D6" s="256"/>
+      <c r="E6" s="256"/>
       <c r="G6" s="138" t="s">
         <v>15</v>
       </c>
@@ -4002,77 +4438,77 @@
       <c r="G7" s="146" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="184"/>
-      <c r="I7" s="185"/>
-      <c r="J7" s="185"/>
-      <c r="K7" s="185"/>
+      <c r="H7" s="259"/>
+      <c r="I7" s="260"/>
+      <c r="J7" s="260"/>
+      <c r="K7" s="260"/>
     </row>
     <row r="8" spans="1:12" s="138" customFormat="1" ht="17.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="146" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="146"/>
-      <c r="C8" s="184"/>
-      <c r="D8" s="184"/>
-      <c r="E8" s="184"/>
+      <c r="C8" s="259"/>
+      <c r="D8" s="259"/>
+      <c r="E8" s="259"/>
       <c r="G8" s="148" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="181"/>
-      <c r="I8" s="182"/>
-      <c r="J8" s="182"/>
-      <c r="K8" s="182"/>
+      <c r="H8" s="256"/>
+      <c r="I8" s="257"/>
+      <c r="J8" s="257"/>
+      <c r="K8" s="257"/>
     </row>
     <row r="9" spans="1:12" s="138" customFormat="1" ht="17.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="148" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="148"/>
-      <c r="C9" s="181"/>
-      <c r="D9" s="181"/>
-      <c r="E9" s="181"/>
+      <c r="C9" s="256"/>
+      <c r="D9" s="256"/>
+      <c r="E9" s="256"/>
       <c r="G9" s="148" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="181"/>
-      <c r="I9" s="182"/>
-      <c r="J9" s="182"/>
-      <c r="K9" s="182"/>
+      <c r="H9" s="256"/>
+      <c r="I9" s="257"/>
+      <c r="J9" s="257"/>
+      <c r="K9" s="257"/>
     </row>
     <row r="10" spans="1:12" s="138" customFormat="1" ht="17.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="148" t="s">
         <v>59</v>
       </c>
       <c r="B10" s="148"/>
-      <c r="C10" s="181"/>
-      <c r="D10" s="181"/>
-      <c r="E10" s="181"/>
+      <c r="C10" s="256"/>
+      <c r="D10" s="256"/>
+      <c r="E10" s="256"/>
       <c r="G10" s="148" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="181"/>
-      <c r="I10" s="182"/>
-      <c r="J10" s="182"/>
-      <c r="K10" s="182"/>
+      <c r="H10" s="256"/>
+      <c r="I10" s="257"/>
+      <c r="J10" s="257"/>
+      <c r="K10" s="257"/>
     </row>
     <row r="11" spans="1:12" s="138" customFormat="1" ht="17.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G11" s="148" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="181"/>
-      <c r="I11" s="182"/>
-      <c r="J11" s="182"/>
-      <c r="K11" s="182"/>
+      <c r="H11" s="256"/>
+      <c r="I11" s="257"/>
+      <c r="J11" s="257"/>
+      <c r="K11" s="257"/>
     </row>
     <row r="12" spans="1:12" s="138" customFormat="1" ht="17.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="152"/>
       <c r="G12" s="148" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="181"/>
-      <c r="I12" s="182"/>
-      <c r="J12" s="182"/>
-      <c r="K12" s="182"/>
+      <c r="H12" s="256"/>
+      <c r="I12" s="257"/>
+      <c r="J12" s="257"/>
+      <c r="K12" s="257"/>
     </row>
     <row r="13" spans="1:12" s="138" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C13" s="152"/>
@@ -4090,86 +4526,86 @@
       <c r="E14" s="155"/>
       <c r="F14" s="155"/>
       <c r="G14" s="138"/>
-      <c r="H14" s="186" t="s">
+      <c r="H14" s="230" t="s">
         <v>26</v>
       </c>
-      <c r="I14" s="187"/>
-      <c r="J14" s="188" t="s">
+      <c r="I14" s="231"/>
+      <c r="J14" s="232" t="s">
         <v>60</v>
       </c>
-      <c r="K14" s="189"/>
-      <c r="L14" s="190"/>
+      <c r="K14" s="233"/>
+      <c r="L14" s="234"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="191" t="s">
+      <c r="A15" s="235" t="s">
         <v>113</v>
       </c>
-      <c r="B15" s="195" t="s">
+      <c r="B15" s="239" t="s">
         <v>114</v>
       </c>
-      <c r="C15" s="196"/>
-      <c r="D15" s="196"/>
-      <c r="E15" s="196"/>
-      <c r="F15" s="196"/>
-      <c r="G15" s="196"/>
-      <c r="H15" s="199"/>
-      <c r="I15" s="200"/>
-      <c r="J15" s="205" t="s">
+      <c r="C15" s="240"/>
+      <c r="D15" s="240"/>
+      <c r="E15" s="240"/>
+      <c r="F15" s="240"/>
+      <c r="G15" s="240"/>
+      <c r="H15" s="243"/>
+      <c r="I15" s="244"/>
+      <c r="J15" s="249" t="s">
         <v>115</v>
       </c>
-      <c r="K15" s="208">
+      <c r="K15" s="251">
         <f>SUM(B20:G20)/6</f>
         <v>0</v>
       </c>
-      <c r="L15" s="210">
+      <c r="L15" s="253">
         <f>ROUND(K15*0.6,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="192"/>
-      <c r="B16" s="197"/>
-      <c r="C16" s="198"/>
-      <c r="D16" s="198"/>
-      <c r="E16" s="198"/>
-      <c r="F16" s="198"/>
-      <c r="G16" s="198"/>
-      <c r="H16" s="201"/>
-      <c r="I16" s="202"/>
-      <c r="J16" s="206"/>
-      <c r="K16" s="209"/>
-      <c r="L16" s="211"/>
+      <c r="A16" s="236"/>
+      <c r="B16" s="241"/>
+      <c r="C16" s="242"/>
+      <c r="D16" s="242"/>
+      <c r="E16" s="242"/>
+      <c r="F16" s="242"/>
+      <c r="G16" s="242"/>
+      <c r="H16" s="245"/>
+      <c r="I16" s="246"/>
+      <c r="J16" s="217"/>
+      <c r="K16" s="252"/>
+      <c r="L16" s="254"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="192"/>
-      <c r="B17" s="197"/>
-      <c r="C17" s="198"/>
-      <c r="D17" s="198"/>
-      <c r="E17" s="198"/>
-      <c r="F17" s="198"/>
-      <c r="G17" s="198"/>
-      <c r="H17" s="201"/>
-      <c r="I17" s="202"/>
-      <c r="J17" s="206"/>
-      <c r="K17" s="209"/>
-      <c r="L17" s="211"/>
+      <c r="A17" s="236"/>
+      <c r="B17" s="241"/>
+      <c r="C17" s="242"/>
+      <c r="D17" s="242"/>
+      <c r="E17" s="242"/>
+      <c r="F17" s="242"/>
+      <c r="G17" s="242"/>
+      <c r="H17" s="245"/>
+      <c r="I17" s="246"/>
+      <c r="J17" s="217"/>
+      <c r="K17" s="252"/>
+      <c r="L17" s="254"/>
     </row>
     <row r="18" spans="1:12" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="192"/>
-      <c r="B18" s="197"/>
-      <c r="C18" s="198"/>
-      <c r="D18" s="198"/>
-      <c r="E18" s="198"/>
-      <c r="F18" s="198"/>
-      <c r="G18" s="198"/>
-      <c r="H18" s="201"/>
-      <c r="I18" s="202"/>
-      <c r="J18" s="206"/>
-      <c r="K18" s="209"/>
-      <c r="L18" s="211"/>
+      <c r="A18" s="236"/>
+      <c r="B18" s="241"/>
+      <c r="C18" s="242"/>
+      <c r="D18" s="242"/>
+      <c r="E18" s="242"/>
+      <c r="F18" s="242"/>
+      <c r="G18" s="242"/>
+      <c r="H18" s="245"/>
+      <c r="I18" s="246"/>
+      <c r="J18" s="217"/>
+      <c r="K18" s="252"/>
+      <c r="L18" s="254"/>
     </row>
     <row r="19" spans="1:12" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="193"/>
+      <c r="A19" s="237"/>
       <c r="B19" s="156" t="s">
         <v>116</v>
       </c>
@@ -4188,148 +4624,148 @@
       <c r="G19" s="159" t="s">
         <v>121</v>
       </c>
-      <c r="H19" s="201"/>
-      <c r="I19" s="202"/>
-      <c r="J19" s="206"/>
-      <c r="K19" s="209"/>
-      <c r="L19" s="211"/>
+      <c r="H19" s="245"/>
+      <c r="I19" s="246"/>
+      <c r="J19" s="217"/>
+      <c r="K19" s="252"/>
+      <c r="L19" s="254"/>
     </row>
     <row r="20" spans="1:12" ht="28.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="194"/>
+      <c r="A20" s="238"/>
       <c r="B20" s="160"/>
       <c r="C20" s="161"/>
       <c r="D20" s="161"/>
       <c r="E20" s="161"/>
       <c r="F20" s="161"/>
       <c r="G20" s="162"/>
-      <c r="H20" s="203"/>
-      <c r="I20" s="204"/>
-      <c r="J20" s="207"/>
-      <c r="K20" s="209"/>
-      <c r="L20" s="212"/>
+      <c r="H20" s="247"/>
+      <c r="I20" s="248"/>
+      <c r="J20" s="250"/>
+      <c r="K20" s="252"/>
+      <c r="L20" s="255"/>
     </row>
     <row r="21" spans="1:12" ht="12.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="217"/>
-      <c r="B21" s="220" t="s">
+      <c r="A21" s="194"/>
+      <c r="B21" s="197" t="s">
         <v>136</v>
       </c>
-      <c r="C21" s="220"/>
-      <c r="D21" s="220"/>
-      <c r="E21" s="220"/>
-      <c r="F21" s="220"/>
-      <c r="G21" s="220"/>
-      <c r="H21" s="222"/>
-      <c r="I21" s="223"/>
-      <c r="J21" s="228" t="s">
+      <c r="C21" s="197"/>
+      <c r="D21" s="197"/>
+      <c r="E21" s="197"/>
+      <c r="F21" s="197"/>
+      <c r="G21" s="197"/>
+      <c r="H21" s="199"/>
+      <c r="I21" s="200"/>
+      <c r="J21" s="205" t="s">
         <v>7</v>
       </c>
-      <c r="K21" s="249">
+      <c r="K21" s="227">
         <f>SUMPRODUCT(B26:G26,B25:G25)</f>
         <v>0</v>
       </c>
-      <c r="L21" s="231">
+      <c r="L21" s="208">
         <f>IF((K21-K28)&gt;=0,ROUND((K21-K28)*0.25,3),0.000000000001)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="218"/>
-      <c r="B22" s="221"/>
-      <c r="C22" s="221"/>
-      <c r="D22" s="221"/>
-      <c r="E22" s="221"/>
-      <c r="F22" s="221"/>
-      <c r="G22" s="221"/>
-      <c r="H22" s="224"/>
-      <c r="I22" s="225"/>
-      <c r="J22" s="229"/>
-      <c r="K22" s="250"/>
-      <c r="L22" s="232"/>
+      <c r="A22" s="195"/>
+      <c r="B22" s="198"/>
+      <c r="C22" s="198"/>
+      <c r="D22" s="198"/>
+      <c r="E22" s="198"/>
+      <c r="F22" s="198"/>
+      <c r="G22" s="198"/>
+      <c r="H22" s="201"/>
+      <c r="I22" s="202"/>
+      <c r="J22" s="206"/>
+      <c r="K22" s="228"/>
+      <c r="L22" s="209"/>
     </row>
     <row r="23" spans="1:12" ht="53" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="218"/>
-      <c r="B23" s="221"/>
-      <c r="C23" s="221"/>
-      <c r="D23" s="221"/>
-      <c r="E23" s="221"/>
-      <c r="F23" s="221"/>
-      <c r="G23" s="221"/>
-      <c r="H23" s="224"/>
-      <c r="I23" s="225"/>
-      <c r="J23" s="229"/>
-      <c r="K23" s="250"/>
-      <c r="L23" s="232"/>
+      <c r="A23" s="195"/>
+      <c r="B23" s="198"/>
+      <c r="C23" s="198"/>
+      <c r="D23" s="198"/>
+      <c r="E23" s="198"/>
+      <c r="F23" s="198"/>
+      <c r="G23" s="198"/>
+      <c r="H23" s="201"/>
+      <c r="I23" s="202"/>
+      <c r="J23" s="206"/>
+      <c r="K23" s="228"/>
+      <c r="L23" s="209"/>
     </row>
     <row r="24" spans="1:12" ht="15.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="218"/>
-      <c r="B24" s="241" t="s">
+      <c r="A24" s="195"/>
+      <c r="B24" s="219" t="s">
         <v>133</v>
       </c>
-      <c r="C24" s="242"/>
-      <c r="D24" s="243" t="s">
+      <c r="C24" s="220"/>
+      <c r="D24" s="221" t="s">
         <v>134</v>
       </c>
-      <c r="E24" s="244"/>
-      <c r="F24" s="245" t="s">
+      <c r="E24" s="222"/>
+      <c r="F24" s="223" t="s">
         <v>135</v>
       </c>
-      <c r="G24" s="246"/>
-      <c r="H24" s="224"/>
-      <c r="I24" s="225"/>
-      <c r="J24" s="229"/>
-      <c r="K24" s="250"/>
-      <c r="L24" s="232"/>
+      <c r="G24" s="224"/>
+      <c r="H24" s="201"/>
+      <c r="I24" s="202"/>
+      <c r="J24" s="206"/>
+      <c r="K24" s="228"/>
+      <c r="L24" s="209"/>
     </row>
     <row r="25" spans="1:12" ht="13.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="218"/>
-      <c r="B25" s="247">
+      <c r="A25" s="195"/>
+      <c r="B25" s="225">
         <v>0.5</v>
       </c>
-      <c r="C25" s="248"/>
-      <c r="D25" s="252">
+      <c r="C25" s="226"/>
+      <c r="D25" s="181">
         <v>0.25</v>
       </c>
-      <c r="E25" s="253"/>
-      <c r="F25" s="254">
+      <c r="E25" s="182"/>
+      <c r="F25" s="183">
         <v>0.25</v>
       </c>
-      <c r="G25" s="255"/>
-      <c r="H25" s="224"/>
-      <c r="I25" s="225"/>
-      <c r="J25" s="229"/>
-      <c r="K25" s="250"/>
-      <c r="L25" s="232"/>
+      <c r="G25" s="184"/>
+      <c r="H25" s="201"/>
+      <c r="I25" s="202"/>
+      <c r="J25" s="206"/>
+      <c r="K25" s="228"/>
+      <c r="L25" s="209"/>
     </row>
     <row r="26" spans="1:12" ht="28.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="218"/>
-      <c r="B26" s="256"/>
-      <c r="C26" s="257"/>
-      <c r="D26" s="258"/>
-      <c r="E26" s="259"/>
-      <c r="F26" s="257"/>
-      <c r="G26" s="260"/>
-      <c r="H26" s="224"/>
-      <c r="I26" s="225"/>
-      <c r="J26" s="229"/>
-      <c r="K26" s="251"/>
-      <c r="L26" s="232"/>
+      <c r="A26" s="195"/>
+      <c r="B26" s="185"/>
+      <c r="C26" s="186"/>
+      <c r="D26" s="187"/>
+      <c r="E26" s="188"/>
+      <c r="F26" s="186"/>
+      <c r="G26" s="189"/>
+      <c r="H26" s="201"/>
+      <c r="I26" s="202"/>
+      <c r="J26" s="206"/>
+      <c r="K26" s="229"/>
+      <c r="L26" s="209"/>
     </row>
     <row r="27" spans="1:12" ht="10.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="218"/>
+      <c r="A27" s="195"/>
       <c r="B27" s="177"/>
       <c r="C27" s="178"/>
       <c r="D27" s="179"/>
       <c r="E27" s="179"/>
       <c r="F27" s="178"/>
       <c r="G27" s="180"/>
-      <c r="H27" s="224"/>
-      <c r="I27" s="225"/>
-      <c r="J27" s="229"/>
+      <c r="H27" s="201"/>
+      <c r="I27" s="202"/>
+      <c r="J27" s="206"/>
       <c r="K27" s="176"/>
-      <c r="L27" s="232"/>
+      <c r="L27" s="209"/>
     </row>
     <row r="28" spans="1:12" ht="28.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="219"/>
+      <c r="A28" s="196"/>
       <c r="B28" s="163" t="s">
         <v>122</v>
       </c>
@@ -4338,42 +4774,42 @@
       <c r="E28" s="164"/>
       <c r="F28" s="164"/>
       <c r="G28" s="164"/>
-      <c r="H28" s="226"/>
-      <c r="I28" s="227"/>
-      <c r="J28" s="230"/>
+      <c r="H28" s="203"/>
+      <c r="I28" s="204"/>
+      <c r="J28" s="207"/>
       <c r="K28" s="165">
         <f>SUM(C28:G28)</f>
         <v>0</v>
       </c>
-      <c r="L28" s="233"/>
+      <c r="L28" s="210"/>
     </row>
     <row r="29" spans="1:12" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="217" t="s">
+      <c r="A29" s="194" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="220" t="s">
+      <c r="B29" s="197" t="s">
         <v>137</v>
       </c>
-      <c r="C29" s="234"/>
-      <c r="D29" s="234"/>
-      <c r="E29" s="234"/>
-      <c r="F29" s="234"/>
-      <c r="G29" s="235"/>
-      <c r="H29" s="236"/>
-      <c r="I29" s="237"/>
-      <c r="J29" s="206" t="s">
+      <c r="C29" s="211"/>
+      <c r="D29" s="211"/>
+      <c r="E29" s="211"/>
+      <c r="F29" s="211"/>
+      <c r="G29" s="212"/>
+      <c r="H29" s="213"/>
+      <c r="I29" s="214"/>
+      <c r="J29" s="217" t="s">
         <v>123</v>
       </c>
       <c r="K29" s="166">
         <v>0</v>
       </c>
-      <c r="L29" s="213">
+      <c r="L29" s="190">
         <f>IF((K29-K30)&gt;=0,ROUND((K29-K30)*0.15,3),0.00000000001)</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="28.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="219"/>
+      <c r="A30" s="196"/>
       <c r="B30" s="167" t="s">
         <v>122</v>
       </c>
@@ -4382,14 +4818,14 @@
       <c r="E30" s="164"/>
       <c r="F30" s="164"/>
       <c r="G30" s="164"/>
-      <c r="H30" s="238"/>
-      <c r="I30" s="239"/>
-      <c r="J30" s="240"/>
+      <c r="H30" s="215"/>
+      <c r="I30" s="216"/>
+      <c r="J30" s="218"/>
       <c r="K30" s="165">
         <f>SUM(C30:G30)</f>
         <v>0</v>
       </c>
-      <c r="L30" s="214"/>
+      <c r="L30" s="191"/>
     </row>
     <row r="31" spans="1:12" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="44"/>
@@ -4407,11 +4843,11 @@
         <v>9</v>
       </c>
       <c r="J32" s="46"/>
-      <c r="K32" s="215">
+      <c r="K32" s="192">
         <f>SUM(L15:L29)</f>
         <v>0</v>
       </c>
-      <c r="L32" s="216"/>
+      <c r="L32" s="193"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="169" t="s">
@@ -4433,11 +4869,26 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="B15:G18"/>
+    <mergeCell ref="H15:I20"/>
+    <mergeCell ref="J15:J20"/>
+    <mergeCell ref="K15:K20"/>
+    <mergeCell ref="L15:L20"/>
     <mergeCell ref="L29:L30"/>
     <mergeCell ref="K32:L32"/>
     <mergeCell ref="A21:A28"/>
@@ -4454,26 +4905,11 @@
     <mergeCell ref="F24:G24"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="K21:K26"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="B15:G18"/>
-    <mergeCell ref="H15:I20"/>
-    <mergeCell ref="J15:J20"/>
-    <mergeCell ref="K15:K20"/>
-    <mergeCell ref="L15:L20"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Endast siffror giltiga" error="Ej giltig siffra_x000a_Kan du ha skrivit komma  istället för punkt eller tvärt om" sqref="C30:G30 C28 D28 E28 F28 G28 F26:G26 D26:E26 B26:C26 K29 B20 C20 D20 E20 F20 G20" xr:uid="{717696C7-3684-477B-A49A-9E6458A0FA01}">
@@ -4560,10 +4996,10 @@
         <v>12</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" s="268"/>
-      <c r="D5" s="268"/>
-      <c r="E5" s="268"/>
-      <c r="F5" s="268"/>
+      <c r="C5" s="261"/>
+      <c r="D5" s="261"/>
+      <c r="E5" s="261"/>
+      <c r="F5" s="261"/>
       <c r="H5" s="9"/>
       <c r="I5" s="13" t="s">
         <v>10</v>
@@ -4577,10 +5013,10 @@
         <v>13</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="268"/>
-      <c r="D6" s="268"/>
-      <c r="E6" s="268"/>
-      <c r="F6" s="268"/>
+      <c r="C6" s="261"/>
+      <c r="D6" s="261"/>
+      <c r="E6" s="261"/>
+      <c r="F6" s="261"/>
       <c r="H6" s="1" t="s">
         <v>15</v>
       </c>
@@ -4597,79 +5033,79 @@
       <c r="H7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="271"/>
-      <c r="J7" s="272"/>
-      <c r="K7" s="272"/>
-      <c r="L7" s="273"/>
+      <c r="I7" s="266"/>
+      <c r="J7" s="267"/>
+      <c r="K7" s="267"/>
+      <c r="L7" s="268"/>
     </row>
     <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="271"/>
-      <c r="D8" s="271"/>
-      <c r="E8" s="271"/>
-      <c r="F8" s="271"/>
+      <c r="C8" s="266"/>
+      <c r="D8" s="266"/>
+      <c r="E8" s="266"/>
+      <c r="F8" s="266"/>
       <c r="H8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="268"/>
-      <c r="J8" s="269"/>
-      <c r="K8" s="269"/>
-      <c r="L8" s="270"/>
+      <c r="I8" s="261"/>
+      <c r="J8" s="262"/>
+      <c r="K8" s="262"/>
+      <c r="L8" s="263"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="12"/>
-      <c r="C9" s="268"/>
-      <c r="D9" s="268"/>
-      <c r="E9" s="268"/>
-      <c r="F9" s="268"/>
+      <c r="C9" s="261"/>
+      <c r="D9" s="261"/>
+      <c r="E9" s="261"/>
+      <c r="F9" s="261"/>
       <c r="H9" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="268"/>
-      <c r="J9" s="269"/>
-      <c r="K9" s="269"/>
-      <c r="L9" s="270"/>
+      <c r="I9" s="261"/>
+      <c r="J9" s="262"/>
+      <c r="K9" s="262"/>
+      <c r="L9" s="263"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>59</v>
       </c>
       <c r="B10" s="12"/>
-      <c r="C10" s="268"/>
-      <c r="D10" s="268"/>
-      <c r="E10" s="268"/>
-      <c r="F10" s="268"/>
+      <c r="C10" s="261"/>
+      <c r="D10" s="261"/>
+      <c r="E10" s="261"/>
+      <c r="F10" s="261"/>
       <c r="H10" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="268"/>
-      <c r="J10" s="269"/>
-      <c r="K10" s="269"/>
-      <c r="L10" s="270"/>
+      <c r="I10" s="261"/>
+      <c r="J10" s="262"/>
+      <c r="K10" s="262"/>
+      <c r="L10" s="263"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="268"/>
-      <c r="J11" s="269"/>
-      <c r="K11" s="269"/>
-      <c r="L11" s="270"/>
+      <c r="I11" s="261"/>
+      <c r="J11" s="262"/>
+      <c r="K11" s="262"/>
+      <c r="L11" s="263"/>
     </row>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H12" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="268"/>
-      <c r="J12" s="269"/>
-      <c r="K12" s="269"/>
-      <c r="L12" s="270"/>
+      <c r="I12" s="261"/>
+      <c r="J12" s="262"/>
+      <c r="K12" s="262"/>
+      <c r="L12" s="263"/>
     </row>
     <row r="13" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15"/>
@@ -4699,12 +5135,12 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="261"/>
-      <c r="B15" s="262" t="s">
+      <c r="A15" s="271"/>
+      <c r="B15" s="272" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="263"/>
-      <c r="D15" s="263"/>
+      <c r="C15" s="265"/>
+      <c r="D15" s="265"/>
       <c r="E15" s="18"/>
       <c r="F15" s="127"/>
       <c r="G15" s="127"/>
@@ -4718,12 +5154,12 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="261"/>
+      <c r="A16" s="271"/>
       <c r="B16" s="264" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="263"/>
-      <c r="D16" s="263"/>
+      <c r="C16" s="265"/>
+      <c r="D16" s="265"/>
       <c r="E16" s="18"/>
       <c r="F16" s="127"/>
       <c r="G16" s="127"/>
@@ -4740,8 +5176,8 @@
       <c r="B17" s="264" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="263"/>
-      <c r="D17" s="263"/>
+      <c r="C17" s="265"/>
+      <c r="D17" s="265"/>
       <c r="E17" s="18"/>
       <c r="F17" s="127"/>
       <c r="G17" s="127"/>
@@ -4755,11 +5191,11 @@
       </c>
     </row>
     <row r="18" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="274" t="s">
+      <c r="B18" s="269" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="275"/>
-      <c r="D18" s="275"/>
+      <c r="C18" s="270"/>
+      <c r="D18" s="270"/>
       <c r="E18" s="18"/>
       <c r="F18" s="127"/>
       <c r="G18" s="127"/>
@@ -4776,8 +5212,8 @@
       <c r="B19" s="264" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="263"/>
-      <c r="D19" s="263"/>
+      <c r="C19" s="265"/>
+      <c r="D19" s="265"/>
       <c r="E19" s="20"/>
       <c r="F19" s="127"/>
       <c r="G19" s="127"/>
@@ -4827,12 +5263,12 @@
       </c>
     </row>
     <row r="22" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="265" t="s">
+      <c r="B22" s="273" t="s">
         <v>104</v>
       </c>
-      <c r="C22" s="266"/>
-      <c r="D22" s="266"/>
-      <c r="E22" s="267"/>
+      <c r="C22" s="274"/>
+      <c r="D22" s="274"/>
+      <c r="E22" s="275"/>
       <c r="F22" s="127"/>
       <c r="G22" s="127"/>
       <c r="H22" s="127"/>
@@ -4956,6 +5392,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B22:E22"/>
     <mergeCell ref="I12:L12"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="C8:F8"/>
@@ -4969,11 +5410,6 @@
     <mergeCell ref="I10:L10"/>
     <mergeCell ref="I11:L11"/>
     <mergeCell ref="C6:F6"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B22:E22"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5056,10 +5492,10 @@
         <v>12</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" s="268"/>
-      <c r="D5" s="268"/>
-      <c r="E5" s="268"/>
-      <c r="F5" s="268"/>
+      <c r="C5" s="261"/>
+      <c r="D5" s="261"/>
+      <c r="E5" s="261"/>
+      <c r="F5" s="261"/>
       <c r="H5" s="9"/>
       <c r="I5" s="13" t="s">
         <v>10</v>
@@ -5073,10 +5509,10 @@
         <v>13</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="268"/>
-      <c r="D6" s="268"/>
-      <c r="E6" s="268"/>
-      <c r="F6" s="268"/>
+      <c r="C6" s="261"/>
+      <c r="D6" s="261"/>
+      <c r="E6" s="261"/>
+      <c r="F6" s="261"/>
       <c r="H6" s="1" t="s">
         <v>15</v>
       </c>
@@ -5093,80 +5529,80 @@
       <c r="H7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="271"/>
-      <c r="J7" s="272"/>
-      <c r="K7" s="272"/>
-      <c r="L7" s="272"/>
+      <c r="I7" s="266"/>
+      <c r="J7" s="267"/>
+      <c r="K7" s="267"/>
+      <c r="L7" s="267"/>
     </row>
     <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="271"/>
-      <c r="D8" s="271"/>
-      <c r="E8" s="271"/>
-      <c r="F8" s="271"/>
+      <c r="C8" s="266"/>
+      <c r="D8" s="266"/>
+      <c r="E8" s="266"/>
+      <c r="F8" s="266"/>
       <c r="H8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="268"/>
-      <c r="J8" s="269"/>
-      <c r="K8" s="269"/>
-      <c r="L8" s="269"/>
+      <c r="I8" s="261"/>
+      <c r="J8" s="262"/>
+      <c r="K8" s="262"/>
+      <c r="L8" s="262"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="12"/>
-      <c r="C9" s="268"/>
-      <c r="D9" s="268"/>
-      <c r="E9" s="268"/>
-      <c r="F9" s="268"/>
+      <c r="C9" s="261"/>
+      <c r="D9" s="261"/>
+      <c r="E9" s="261"/>
+      <c r="F9" s="261"/>
       <c r="H9" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="268"/>
-      <c r="J9" s="269"/>
-      <c r="K9" s="269"/>
-      <c r="L9" s="269"/>
+      <c r="I9" s="261"/>
+      <c r="J9" s="262"/>
+      <c r="K9" s="262"/>
+      <c r="L9" s="262"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>59</v>
       </c>
       <c r="B10" s="12"/>
-      <c r="C10" s="268"/>
-      <c r="D10" s="268"/>
-      <c r="E10" s="268"/>
-      <c r="F10" s="268"/>
+      <c r="C10" s="261"/>
+      <c r="D10" s="261"/>
+      <c r="E10" s="261"/>
+      <c r="F10" s="261"/>
       <c r="H10" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="268"/>
-      <c r="J10" s="269"/>
-      <c r="K10" s="269"/>
-      <c r="L10" s="269"/>
+      <c r="I10" s="261"/>
+      <c r="J10" s="262"/>
+      <c r="K10" s="262"/>
+      <c r="L10" s="262"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="268"/>
-      <c r="J11" s="269"/>
-      <c r="K11" s="269"/>
-      <c r="L11" s="269"/>
+      <c r="I11" s="261"/>
+      <c r="J11" s="262"/>
+      <c r="K11" s="262"/>
+      <c r="L11" s="262"/>
     </row>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="14"/>
       <c r="H12" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="268"/>
-      <c r="J12" s="269"/>
-      <c r="K12" s="269"/>
-      <c r="L12" s="269"/>
+      <c r="I12" s="261"/>
+      <c r="J12" s="262"/>
+      <c r="K12" s="262"/>
+      <c r="L12" s="262"/>
     </row>
     <row r="13" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H13" s="3"/>
@@ -5203,12 +5639,12 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="261"/>
-      <c r="B16" s="262" t="s">
+      <c r="A16" s="271"/>
+      <c r="B16" s="272" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="263"/>
-      <c r="D16" s="263"/>
+      <c r="C16" s="265"/>
+      <c r="D16" s="265"/>
       <c r="E16" s="18"/>
       <c r="F16" s="127"/>
       <c r="G16" s="127"/>
@@ -5222,12 +5658,12 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="261"/>
+      <c r="A17" s="271"/>
       <c r="B17" s="264" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="263"/>
-      <c r="D17" s="263"/>
+      <c r="C17" s="265"/>
+      <c r="D17" s="265"/>
       <c r="E17" s="18"/>
       <c r="F17" s="127"/>
       <c r="G17" s="127"/>
@@ -5244,8 +5680,8 @@
       <c r="B18" s="264" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="263"/>
-      <c r="D18" s="263"/>
+      <c r="C18" s="265"/>
+      <c r="D18" s="265"/>
       <c r="E18" s="18"/>
       <c r="F18" s="127"/>
       <c r="G18" s="127"/>
@@ -5262,8 +5698,8 @@
       <c r="B19" s="276" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="263"/>
-      <c r="D19" s="263"/>
+      <c r="C19" s="265"/>
+      <c r="D19" s="265"/>
       <c r="E19" s="18"/>
       <c r="F19" s="127"/>
       <c r="G19" s="127"/>
@@ -5280,8 +5716,8 @@
       <c r="B20" s="264" t="s">
         <v>102</v>
       </c>
-      <c r="C20" s="263"/>
-      <c r="D20" s="263"/>
+      <c r="C20" s="265"/>
+      <c r="D20" s="265"/>
       <c r="E20" s="277"/>
       <c r="F20" s="127"/>
       <c r="G20" s="127"/>
@@ -5298,8 +5734,8 @@
       <c r="B21" s="264" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="263"/>
-      <c r="D21" s="263"/>
+      <c r="C21" s="265"/>
+      <c r="D21" s="265"/>
       <c r="E21" s="18"/>
       <c r="F21" s="127"/>
       <c r="G21" s="127"/>
@@ -5313,12 +5749,12 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="265" t="s">
+      <c r="B22" s="273" t="s">
         <v>103</v>
       </c>
-      <c r="C22" s="266"/>
-      <c r="D22" s="266"/>
-      <c r="E22" s="267"/>
+      <c r="C22" s="274"/>
+      <c r="D22" s="274"/>
+      <c r="E22" s="275"/>
       <c r="F22" s="127"/>
       <c r="G22" s="127"/>
       <c r="H22" s="127"/>
@@ -5471,6 +5907,13 @@
     <row r="66" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:E20"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="I8:L8"/>
@@ -5483,13 +5926,6 @@
     <mergeCell ref="I10:L10"/>
     <mergeCell ref="I11:L11"/>
     <mergeCell ref="C9:F9"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="I12:L12"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:E20"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5575,10 +6011,10 @@
         <v>12</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" s="268"/>
-      <c r="D5" s="268"/>
-      <c r="E5" s="268"/>
-      <c r="F5" s="268"/>
+      <c r="C5" s="261"/>
+      <c r="D5" s="261"/>
+      <c r="E5" s="261"/>
+      <c r="F5" s="261"/>
       <c r="H5" s="9"/>
       <c r="I5" s="13" t="s">
         <v>10</v>
@@ -5592,10 +6028,10 @@
         <v>13</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="268"/>
-      <c r="D6" s="268"/>
-      <c r="E6" s="268"/>
-      <c r="F6" s="268"/>
+      <c r="C6" s="261"/>
+      <c r="D6" s="261"/>
+      <c r="E6" s="261"/>
+      <c r="F6" s="261"/>
       <c r="H6" s="1" t="s">
         <v>15</v>
       </c>
@@ -5612,80 +6048,80 @@
       <c r="H7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="271"/>
-      <c r="J7" s="272"/>
-      <c r="K7" s="272"/>
-      <c r="L7" s="273"/>
+      <c r="I7" s="266"/>
+      <c r="J7" s="267"/>
+      <c r="K7" s="267"/>
+      <c r="L7" s="268"/>
     </row>
     <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="271"/>
-      <c r="D8" s="271"/>
-      <c r="E8" s="271"/>
-      <c r="F8" s="271"/>
+      <c r="C8" s="266"/>
+      <c r="D8" s="266"/>
+      <c r="E8" s="266"/>
+      <c r="F8" s="266"/>
       <c r="H8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="268"/>
-      <c r="J8" s="269"/>
-      <c r="K8" s="269"/>
-      <c r="L8" s="270"/>
+      <c r="I8" s="261"/>
+      <c r="J8" s="262"/>
+      <c r="K8" s="262"/>
+      <c r="L8" s="263"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="12"/>
-      <c r="C9" s="268"/>
-      <c r="D9" s="268"/>
-      <c r="E9" s="268"/>
-      <c r="F9" s="268"/>
+      <c r="C9" s="261"/>
+      <c r="D9" s="261"/>
+      <c r="E9" s="261"/>
+      <c r="F9" s="261"/>
       <c r="H9" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="268"/>
-      <c r="J9" s="269"/>
-      <c r="K9" s="269"/>
-      <c r="L9" s="270"/>
+      <c r="I9" s="261"/>
+      <c r="J9" s="262"/>
+      <c r="K9" s="262"/>
+      <c r="L9" s="263"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>59</v>
       </c>
       <c r="B10" s="12"/>
-      <c r="C10" s="268"/>
-      <c r="D10" s="268"/>
-      <c r="E10" s="268"/>
-      <c r="F10" s="268"/>
+      <c r="C10" s="261"/>
+      <c r="D10" s="261"/>
+      <c r="E10" s="261"/>
+      <c r="F10" s="261"/>
       <c r="H10" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="268"/>
-      <c r="J10" s="269"/>
-      <c r="K10" s="269"/>
-      <c r="L10" s="270"/>
+      <c r="I10" s="261"/>
+      <c r="J10" s="262"/>
+      <c r="K10" s="262"/>
+      <c r="L10" s="263"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="268"/>
-      <c r="J11" s="269"/>
-      <c r="K11" s="269"/>
-      <c r="L11" s="270"/>
+      <c r="I11" s="261"/>
+      <c r="J11" s="262"/>
+      <c r="K11" s="262"/>
+      <c r="L11" s="263"/>
     </row>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="14"/>
       <c r="H12" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="268"/>
-      <c r="J12" s="269"/>
-      <c r="K12" s="269"/>
-      <c r="L12" s="270"/>
+      <c r="I12" s="261"/>
+      <c r="J12" s="262"/>
+      <c r="K12" s="262"/>
+      <c r="L12" s="263"/>
     </row>
     <row r="13" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15"/>
@@ -5715,8 +6151,8 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="261"/>
-      <c r="B15" s="262" t="s">
+      <c r="A15" s="271"/>
+      <c r="B15" s="272" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="278"/>
@@ -5734,12 +6170,12 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="261"/>
+      <c r="A16" s="271"/>
       <c r="B16" s="264" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="263"/>
-      <c r="D16" s="263"/>
+      <c r="C16" s="265"/>
+      <c r="D16" s="265"/>
       <c r="E16" s="277"/>
       <c r="F16" s="127"/>
       <c r="G16" s="127"/>
@@ -5756,8 +6192,8 @@
       <c r="B17" s="264" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="263"/>
-      <c r="D17" s="263"/>
+      <c r="C17" s="265"/>
+      <c r="D17" s="265"/>
       <c r="E17" s="277"/>
       <c r="F17" s="127"/>
       <c r="G17" s="127"/>
@@ -5792,8 +6228,8 @@
       <c r="B19" s="264" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="263"/>
-      <c r="D19" s="263"/>
+      <c r="C19" s="265"/>
+      <c r="D19" s="265"/>
       <c r="E19" s="277"/>
       <c r="F19" s="127"/>
       <c r="G19" s="127"/>
@@ -5810,8 +6246,8 @@
       <c r="B20" s="264" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="263"/>
-      <c r="D20" s="263"/>
+      <c r="C20" s="265"/>
+      <c r="D20" s="265"/>
       <c r="E20" s="277"/>
       <c r="F20" s="127"/>
       <c r="G20" s="127"/>
@@ -5828,8 +6264,8 @@
       <c r="B21" s="264" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="263"/>
-      <c r="D21" s="263"/>
+      <c r="C21" s="265"/>
+      <c r="D21" s="265"/>
       <c r="E21" s="277"/>
       <c r="F21" s="127"/>
       <c r="G21" s="127"/>
@@ -5976,6 +6412,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B18:E18"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="I7:L7"/>
     <mergeCell ref="C6:F6"/>
@@ -5988,14 +6432,6 @@
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="I8:L8"/>
     <mergeCell ref="I12:L12"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B18:E18"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6079,10 +6515,10 @@
         <v>12</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" s="268"/>
-      <c r="D5" s="268"/>
-      <c r="E5" s="268"/>
-      <c r="F5" s="268"/>
+      <c r="C5" s="261"/>
+      <c r="D5" s="261"/>
+      <c r="E5" s="261"/>
+      <c r="F5" s="261"/>
       <c r="H5" s="9"/>
       <c r="I5" s="13" t="s">
         <v>10</v>
@@ -6096,10 +6532,10 @@
         <v>13</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="268"/>
-      <c r="D6" s="268"/>
-      <c r="E6" s="268"/>
-      <c r="F6" s="268"/>
+      <c r="C6" s="261"/>
+      <c r="D6" s="261"/>
+      <c r="E6" s="261"/>
+      <c r="F6" s="261"/>
       <c r="H6" s="1" t="s">
         <v>15</v>
       </c>
@@ -6116,79 +6552,79 @@
       <c r="H7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="271"/>
-      <c r="J7" s="272"/>
-      <c r="K7" s="272"/>
-      <c r="L7" s="273"/>
+      <c r="I7" s="266"/>
+      <c r="J7" s="267"/>
+      <c r="K7" s="267"/>
+      <c r="L7" s="268"/>
     </row>
     <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="271"/>
-      <c r="D8" s="271"/>
-      <c r="E8" s="271"/>
-      <c r="F8" s="271"/>
+      <c r="C8" s="266"/>
+      <c r="D8" s="266"/>
+      <c r="E8" s="266"/>
+      <c r="F8" s="266"/>
       <c r="H8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="268"/>
-      <c r="J8" s="269"/>
-      <c r="K8" s="269"/>
-      <c r="L8" s="270"/>
+      <c r="I8" s="261"/>
+      <c r="J8" s="262"/>
+      <c r="K8" s="262"/>
+      <c r="L8" s="263"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="12"/>
-      <c r="C9" s="268"/>
-      <c r="D9" s="268"/>
-      <c r="E9" s="268"/>
-      <c r="F9" s="268"/>
+      <c r="C9" s="261"/>
+      <c r="D9" s="261"/>
+      <c r="E9" s="261"/>
+      <c r="F9" s="261"/>
       <c r="H9" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="268"/>
-      <c r="J9" s="269"/>
-      <c r="K9" s="269"/>
-      <c r="L9" s="270"/>
+      <c r="I9" s="261"/>
+      <c r="J9" s="262"/>
+      <c r="K9" s="262"/>
+      <c r="L9" s="263"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>59</v>
       </c>
       <c r="B10" s="12"/>
-      <c r="C10" s="268"/>
-      <c r="D10" s="268"/>
-      <c r="E10" s="268"/>
-      <c r="F10" s="268"/>
+      <c r="C10" s="261"/>
+      <c r="D10" s="261"/>
+      <c r="E10" s="261"/>
+      <c r="F10" s="261"/>
       <c r="H10" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="268"/>
-      <c r="J10" s="269"/>
-      <c r="K10" s="269"/>
-      <c r="L10" s="270"/>
+      <c r="I10" s="261"/>
+      <c r="J10" s="262"/>
+      <c r="K10" s="262"/>
+      <c r="L10" s="263"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="268"/>
-      <c r="J11" s="269"/>
-      <c r="K11" s="269"/>
-      <c r="L11" s="270"/>
+      <c r="I11" s="261"/>
+      <c r="J11" s="262"/>
+      <c r="K11" s="262"/>
+      <c r="L11" s="263"/>
     </row>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H12" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="268"/>
-      <c r="J12" s="269"/>
-      <c r="K12" s="269"/>
-      <c r="L12" s="270"/>
+      <c r="I12" s="261"/>
+      <c r="J12" s="262"/>
+      <c r="K12" s="262"/>
+      <c r="L12" s="263"/>
     </row>
     <row r="13" spans="1:12" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H13" s="3"/>
@@ -6565,10 +7001,10 @@
         <v>12</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" s="268"/>
-      <c r="D5" s="268"/>
-      <c r="E5" s="268"/>
-      <c r="F5" s="268"/>
+      <c r="C5" s="261"/>
+      <c r="D5" s="261"/>
+      <c r="E5" s="261"/>
+      <c r="F5" s="261"/>
       <c r="H5" s="9"/>
       <c r="I5" s="13" t="s">
         <v>10</v>
@@ -6582,10 +7018,10 @@
         <v>13</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="268"/>
-      <c r="D6" s="268"/>
-      <c r="E6" s="268"/>
-      <c r="F6" s="268"/>
+      <c r="C6" s="261"/>
+      <c r="D6" s="261"/>
+      <c r="E6" s="261"/>
+      <c r="F6" s="261"/>
       <c r="H6" s="1" t="s">
         <v>15</v>
       </c>
@@ -6602,79 +7038,79 @@
       <c r="H7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="271"/>
-      <c r="J7" s="272"/>
-      <c r="K7" s="272"/>
-      <c r="L7" s="273"/>
+      <c r="I7" s="266"/>
+      <c r="J7" s="267"/>
+      <c r="K7" s="267"/>
+      <c r="L7" s="268"/>
     </row>
     <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="271"/>
-      <c r="D8" s="271"/>
-      <c r="E8" s="271"/>
-      <c r="F8" s="271"/>
+      <c r="C8" s="266"/>
+      <c r="D8" s="266"/>
+      <c r="E8" s="266"/>
+      <c r="F8" s="266"/>
       <c r="H8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="268"/>
-      <c r="J8" s="269"/>
-      <c r="K8" s="269"/>
-      <c r="L8" s="270"/>
+      <c r="I8" s="261"/>
+      <c r="J8" s="262"/>
+      <c r="K8" s="262"/>
+      <c r="L8" s="263"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="12"/>
-      <c r="C9" s="268"/>
-      <c r="D9" s="268"/>
-      <c r="E9" s="268"/>
-      <c r="F9" s="268"/>
+      <c r="C9" s="261"/>
+      <c r="D9" s="261"/>
+      <c r="E9" s="261"/>
+      <c r="F9" s="261"/>
       <c r="H9" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="268"/>
-      <c r="J9" s="269"/>
-      <c r="K9" s="269"/>
-      <c r="L9" s="270"/>
+      <c r="I9" s="261"/>
+      <c r="J9" s="262"/>
+      <c r="K9" s="262"/>
+      <c r="L9" s="263"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>59</v>
       </c>
       <c r="B10" s="12"/>
-      <c r="C10" s="268"/>
-      <c r="D10" s="268"/>
-      <c r="E10" s="268"/>
-      <c r="F10" s="268"/>
+      <c r="C10" s="261"/>
+      <c r="D10" s="261"/>
+      <c r="E10" s="261"/>
+      <c r="F10" s="261"/>
       <c r="H10" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="268"/>
-      <c r="J10" s="269"/>
-      <c r="K10" s="269"/>
-      <c r="L10" s="270"/>
+      <c r="I10" s="261"/>
+      <c r="J10" s="262"/>
+      <c r="K10" s="262"/>
+      <c r="L10" s="263"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="268"/>
-      <c r="J11" s="269"/>
-      <c r="K11" s="269"/>
-      <c r="L11" s="270"/>
+      <c r="I11" s="261"/>
+      <c r="J11" s="262"/>
+      <c r="K11" s="262"/>
+      <c r="L11" s="263"/>
     </row>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H12" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="268"/>
-      <c r="J12" s="269"/>
-      <c r="K12" s="269"/>
-      <c r="L12" s="270"/>
+      <c r="I12" s="261"/>
+      <c r="J12" s="262"/>
+      <c r="K12" s="262"/>
+      <c r="L12" s="263"/>
     </row>
     <row r="13" spans="1:12" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H13" s="3"/>
@@ -6715,17 +7151,17 @@
     </row>
     <row r="16" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="287"/>
-      <c r="B16" s="272"/>
-      <c r="C16" s="272"/>
-      <c r="D16" s="272"/>
-      <c r="E16" s="272"/>
-      <c r="F16" s="272"/>
-      <c r="G16" s="272"/>
-      <c r="H16" s="272"/>
-      <c r="I16" s="272"/>
-      <c r="J16" s="272"/>
-      <c r="K16" s="272"/>
-      <c r="L16" s="273"/>
+      <c r="B16" s="267"/>
+      <c r="C16" s="267"/>
+      <c r="D16" s="267"/>
+      <c r="E16" s="267"/>
+      <c r="F16" s="267"/>
+      <c r="G16" s="267"/>
+      <c r="H16" s="267"/>
+      <c r="I16" s="267"/>
+      <c r="J16" s="267"/>
+      <c r="K16" s="267"/>
+      <c r="L16" s="268"/>
     </row>
     <row r="17" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="107" t="s">
@@ -7088,10 +7524,10 @@
         <v>12</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" s="268"/>
-      <c r="D5" s="268"/>
-      <c r="E5" s="268"/>
-      <c r="F5" s="268"/>
+      <c r="C5" s="261"/>
+      <c r="D5" s="261"/>
+      <c r="E5" s="261"/>
+      <c r="F5" s="261"/>
       <c r="H5" s="9"/>
       <c r="I5" s="13" t="s">
         <v>10</v>
@@ -7105,10 +7541,10 @@
         <v>13</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="268"/>
-      <c r="D6" s="268"/>
-      <c r="E6" s="268"/>
-      <c r="F6" s="268"/>
+      <c r="C6" s="261"/>
+      <c r="D6" s="261"/>
+      <c r="E6" s="261"/>
+      <c r="F6" s="261"/>
       <c r="H6" s="1" t="s">
         <v>15</v>
       </c>
@@ -7125,79 +7561,79 @@
       <c r="H7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="271"/>
-      <c r="J7" s="272"/>
-      <c r="K7" s="272"/>
-      <c r="L7" s="273"/>
+      <c r="I7" s="266"/>
+      <c r="J7" s="267"/>
+      <c r="K7" s="267"/>
+      <c r="L7" s="268"/>
     </row>
     <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="271"/>
-      <c r="D8" s="271"/>
-      <c r="E8" s="271"/>
-      <c r="F8" s="271"/>
+      <c r="C8" s="266"/>
+      <c r="D8" s="266"/>
+      <c r="E8" s="266"/>
+      <c r="F8" s="266"/>
       <c r="H8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="268"/>
-      <c r="J8" s="269"/>
-      <c r="K8" s="269"/>
-      <c r="L8" s="270"/>
+      <c r="I8" s="261"/>
+      <c r="J8" s="262"/>
+      <c r="K8" s="262"/>
+      <c r="L8" s="263"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="12"/>
-      <c r="C9" s="268"/>
-      <c r="D9" s="268"/>
-      <c r="E9" s="268"/>
-      <c r="F9" s="268"/>
+      <c r="C9" s="261"/>
+      <c r="D9" s="261"/>
+      <c r="E9" s="261"/>
+      <c r="F9" s="261"/>
       <c r="H9" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="268"/>
-      <c r="J9" s="269"/>
-      <c r="K9" s="269"/>
-      <c r="L9" s="270"/>
+      <c r="I9" s="261"/>
+      <c r="J9" s="262"/>
+      <c r="K9" s="262"/>
+      <c r="L9" s="263"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>59</v>
       </c>
       <c r="B10" s="12"/>
-      <c r="C10" s="268"/>
-      <c r="D10" s="268"/>
-      <c r="E10" s="268"/>
-      <c r="F10" s="268"/>
+      <c r="C10" s="261"/>
+      <c r="D10" s="261"/>
+      <c r="E10" s="261"/>
+      <c r="F10" s="261"/>
       <c r="H10" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="268"/>
-      <c r="J10" s="269"/>
-      <c r="K10" s="269"/>
-      <c r="L10" s="270"/>
+      <c r="I10" s="261"/>
+      <c r="J10" s="262"/>
+      <c r="K10" s="262"/>
+      <c r="L10" s="263"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="268"/>
-      <c r="J11" s="269"/>
-      <c r="K11" s="269"/>
-      <c r="L11" s="270"/>
+      <c r="I11" s="261"/>
+      <c r="J11" s="262"/>
+      <c r="K11" s="262"/>
+      <c r="L11" s="263"/>
     </row>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H12" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="268"/>
-      <c r="J12" s="269"/>
-      <c r="K12" s="269"/>
-      <c r="L12" s="270"/>
+      <c r="I12" s="261"/>
+      <c r="J12" s="262"/>
+      <c r="K12" s="262"/>
+      <c r="L12" s="263"/>
     </row>
     <row r="13" spans="1:12" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H13" s="3"/>
@@ -7238,17 +7674,17 @@
     </row>
     <row r="16" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="287"/>
-      <c r="B16" s="272"/>
-      <c r="C16" s="272"/>
-      <c r="D16" s="272"/>
-      <c r="E16" s="272"/>
-      <c r="F16" s="272"/>
-      <c r="G16" s="272"/>
-      <c r="H16" s="272"/>
-      <c r="I16" s="272"/>
-      <c r="J16" s="272"/>
-      <c r="K16" s="272"/>
-      <c r="L16" s="273"/>
+      <c r="B16" s="267"/>
+      <c r="C16" s="267"/>
+      <c r="D16" s="267"/>
+      <c r="E16" s="267"/>
+      <c r="F16" s="267"/>
+      <c r="G16" s="267"/>
+      <c r="H16" s="267"/>
+      <c r="I16" s="267"/>
+      <c r="J16" s="267"/>
+      <c r="K16" s="267"/>
+      <c r="L16" s="268"/>
     </row>
     <row r="17" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="107" t="s">
@@ -7581,7 +8017,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView showZeros="0" view="pageLayout" zoomScale="110" zoomScaleNormal="120" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -7647,10 +8083,10 @@
         <v>12</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" s="268"/>
-      <c r="D5" s="268"/>
-      <c r="E5" s="268"/>
-      <c r="F5" s="268"/>
+      <c r="C5" s="261"/>
+      <c r="D5" s="261"/>
+      <c r="E5" s="261"/>
+      <c r="F5" s="261"/>
       <c r="H5" s="9"/>
       <c r="I5" s="13" t="s">
         <v>10</v>
@@ -7664,10 +8100,10 @@
         <v>13</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="268"/>
-      <c r="D6" s="268"/>
-      <c r="E6" s="268"/>
-      <c r="F6" s="268"/>
+      <c r="C6" s="261"/>
+      <c r="D6" s="261"/>
+      <c r="E6" s="261"/>
+      <c r="F6" s="261"/>
       <c r="H6" s="1" t="s">
         <v>15</v>
       </c>
@@ -7684,80 +8120,80 @@
       <c r="H7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="271"/>
-      <c r="J7" s="272"/>
-      <c r="K7" s="272"/>
-      <c r="L7" s="273"/>
+      <c r="I7" s="266"/>
+      <c r="J7" s="267"/>
+      <c r="K7" s="267"/>
+      <c r="L7" s="268"/>
     </row>
     <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="271"/>
-      <c r="D8" s="271"/>
-      <c r="E8" s="271"/>
-      <c r="F8" s="271"/>
+      <c r="C8" s="266"/>
+      <c r="D8" s="266"/>
+      <c r="E8" s="266"/>
+      <c r="F8" s="266"/>
       <c r="H8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="268"/>
-      <c r="J8" s="269"/>
-      <c r="K8" s="269"/>
-      <c r="L8" s="270"/>
+      <c r="I8" s="261"/>
+      <c r="J8" s="262"/>
+      <c r="K8" s="262"/>
+      <c r="L8" s="263"/>
     </row>
     <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="12"/>
-      <c r="C9" s="268"/>
-      <c r="D9" s="268"/>
-      <c r="E9" s="268"/>
-      <c r="F9" s="268"/>
+      <c r="C9" s="261"/>
+      <c r="D9" s="261"/>
+      <c r="E9" s="261"/>
+      <c r="F9" s="261"/>
       <c r="H9" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="268"/>
-      <c r="J9" s="269"/>
-      <c r="K9" s="269"/>
-      <c r="L9" s="270"/>
+      <c r="I9" s="261"/>
+      <c r="J9" s="262"/>
+      <c r="K9" s="262"/>
+      <c r="L9" s="263"/>
     </row>
     <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>59</v>
       </c>
       <c r="B10" s="12"/>
-      <c r="C10" s="268"/>
-      <c r="D10" s="268"/>
-      <c r="E10" s="268"/>
-      <c r="F10" s="268"/>
+      <c r="C10" s="261"/>
+      <c r="D10" s="261"/>
+      <c r="E10" s="261"/>
+      <c r="F10" s="261"/>
       <c r="H10" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="268"/>
-      <c r="J10" s="269"/>
-      <c r="K10" s="269"/>
-      <c r="L10" s="270"/>
+      <c r="I10" s="261"/>
+      <c r="J10" s="262"/>
+      <c r="K10" s="262"/>
+      <c r="L10" s="263"/>
     </row>
     <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="268"/>
-      <c r="J11" s="269"/>
-      <c r="K11" s="269"/>
-      <c r="L11" s="270"/>
+      <c r="I11" s="261"/>
+      <c r="J11" s="262"/>
+      <c r="K11" s="262"/>
+      <c r="L11" s="263"/>
     </row>
     <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="14"/>
       <c r="H12" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="268"/>
-      <c r="J12" s="269"/>
-      <c r="K12" s="269"/>
-      <c r="L12" s="270"/>
+      <c r="I12" s="261"/>
+      <c r="J12" s="262"/>
+      <c r="K12" s="262"/>
+      <c r="L12" s="263"/>
     </row>
     <row r="13" spans="1:13" ht="8.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="14"/>
@@ -7778,16 +8214,16 @@
       <c r="A15" s="172" t="s">
         <v>127</v>
       </c>
-      <c r="B15" s="300" t="s">
+      <c r="B15" s="288" t="s">
         <v>128</v>
       </c>
-      <c r="C15" s="301"/>
-      <c r="D15" s="301"/>
-      <c r="E15" s="301"/>
-      <c r="F15" s="301"/>
-      <c r="G15" s="301"/>
-      <c r="H15" s="301"/>
-      <c r="I15" s="302"/>
+      <c r="C15" s="289"/>
+      <c r="D15" s="289"/>
+      <c r="E15" s="289"/>
+      <c r="F15" s="289"/>
+      <c r="G15" s="289"/>
+      <c r="H15" s="289"/>
+      <c r="I15" s="290"/>
       <c r="J15" s="173" t="s">
         <v>129</v>
       </c>
@@ -7798,41 +8234,41 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="66.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="288" t="s">
+      <c r="A16" s="291" t="s">
         <v>143</v>
       </c>
-      <c r="B16" s="292" t="s">
+      <c r="B16" s="295" t="s">
         <v>141</v>
       </c>
-      <c r="C16" s="293"/>
-      <c r="D16" s="293"/>
-      <c r="E16" s="293"/>
-      <c r="F16" s="293"/>
-      <c r="G16" s="293"/>
-      <c r="H16" s="293"/>
-      <c r="I16" s="293"/>
+      <c r="C16" s="296"/>
+      <c r="D16" s="296"/>
+      <c r="E16" s="296"/>
+      <c r="F16" s="296"/>
+      <c r="G16" s="296"/>
+      <c r="H16" s="296"/>
+      <c r="I16" s="296"/>
       <c r="J16" s="78" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="K16" s="130"/>
       <c r="L16" s="79">
-        <f>K16*0.1</f>
+        <f>K16*0.2</f>
         <v>0</v>
       </c>
       <c r="M16" s="80"/>
     </row>
     <row r="17" spans="1:13" ht="83.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="289"/>
-      <c r="B17" s="292" t="s">
+      <c r="A17" s="292"/>
+      <c r="B17" s="295" t="s">
         <v>142</v>
       </c>
-      <c r="C17" s="293"/>
-      <c r="D17" s="293"/>
-      <c r="E17" s="293"/>
-      <c r="F17" s="293"/>
-      <c r="G17" s="293"/>
-      <c r="H17" s="293"/>
-      <c r="I17" s="293"/>
+      <c r="C17" s="296"/>
+      <c r="D17" s="296"/>
+      <c r="E17" s="296"/>
+      <c r="F17" s="296"/>
+      <c r="G17" s="296"/>
+      <c r="H17" s="296"/>
+      <c r="I17" s="296"/>
       <c r="J17" s="81" t="s">
         <v>130</v>
       </c>
@@ -7844,47 +8280,47 @@
       <c r="M17" s="80"/>
     </row>
     <row r="18" spans="1:13" ht="58.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="290" t="s">
+      <c r="A18" s="293" t="s">
         <v>144</v>
       </c>
-      <c r="B18" s="294" t="s">
+      <c r="B18" s="297" t="s">
         <v>131</v>
       </c>
-      <c r="C18" s="295"/>
-      <c r="D18" s="295"/>
-      <c r="E18" s="295"/>
-      <c r="F18" s="295"/>
-      <c r="G18" s="295"/>
-      <c r="H18" s="295"/>
-      <c r="I18" s="296"/>
+      <c r="C18" s="298"/>
+      <c r="D18" s="298"/>
+      <c r="E18" s="298"/>
+      <c r="F18" s="298"/>
+      <c r="G18" s="298"/>
+      <c r="H18" s="298"/>
+      <c r="I18" s="299"/>
       <c r="J18" s="78" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="K18" s="132"/>
       <c r="L18" s="83">
-        <f>K18*0.3</f>
+        <f>K18*0.25</f>
         <v>0</v>
       </c>
       <c r="M18" s="80"/>
     </row>
     <row r="19" spans="1:13" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="291"/>
-      <c r="B19" s="297" t="s">
+      <c r="A19" s="294"/>
+      <c r="B19" s="300" t="s">
         <v>132</v>
       </c>
-      <c r="C19" s="298"/>
-      <c r="D19" s="298"/>
-      <c r="E19" s="298"/>
-      <c r="F19" s="298"/>
-      <c r="G19" s="298"/>
-      <c r="H19" s="298"/>
-      <c r="I19" s="299"/>
+      <c r="C19" s="301"/>
+      <c r="D19" s="301"/>
+      <c r="E19" s="301"/>
+      <c r="F19" s="301"/>
+      <c r="G19" s="301"/>
+      <c r="H19" s="301"/>
+      <c r="I19" s="302"/>
       <c r="J19" s="84" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="K19" s="133"/>
       <c r="L19" s="85">
-        <f>K19*0.3</f>
+        <f>K19*0.25</f>
         <v>0</v>
       </c>
       <c r="M19" s="80"/>
@@ -7955,6 +8391,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B16:I16"/>
+    <mergeCell ref="B17:I17"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="B19:I19"/>
     <mergeCell ref="B15:I15"/>
     <mergeCell ref="I12:L12"/>
     <mergeCell ref="C5:F5"/>
@@ -7967,12 +8409,6 @@
     <mergeCell ref="I10:L10"/>
     <mergeCell ref="I11:L11"/>
     <mergeCell ref="C6:F6"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B16:I16"/>
-    <mergeCell ref="B17:I17"/>
-    <mergeCell ref="B18:I18"/>
-    <mergeCell ref="B19:I19"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7986,24 +8422,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100570C130F412EDB4EBF3E80DF6A9149FD" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfaa3b10b9be17ef9f56bd19dc71004c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddb0c952b897a810c8a4e377cff6bff8" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -8069,30 +8487,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64838F1D-7ECA-4F32-944F-43492487C498}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A00BD0D-8423-4FFE-92A4-D273D2078383}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8107,4 +8520,27 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64838F1D-7ECA-4F32-944F-43492487C498}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>